<commit_message>
QA edit to SP patient-birthdate  ( no multipleAnd )
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0A5A06-695F-EA49-A999-7B2AC83FC935}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B02235-B0FE-4B9E-884F-706769055530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2267" uniqueCount="794">
   <si>
     <t>Element</t>
   </si>
@@ -2501,7 +2501,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2967,13 +2967,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="105" customHeight="1">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="141" customHeight="1">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="103.5" customHeight="1">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3042,9 +3042,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3065,15 +3065,15 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>381</v>
       </c>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>383</v>
       </c>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>385</v>
       </c>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>386</v>
       </c>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>388</v>
       </c>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>303</v>
       </c>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>391</v>
       </c>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>393</v>
       </c>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>395</v>
       </c>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>397</v>
       </c>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>398</v>
       </c>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>789</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>400</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>402</v>
       </c>
@@ -3312,7 +3312,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>468</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>198</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>406</v>
       </c>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>256</v>
       </c>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>409</v>
       </c>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>411</v>
       </c>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>791</v>
       </c>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>197</v>
       </c>
@@ -3432,7 +3432,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -3464,22 +3464,22 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="17.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>254</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>268</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>272</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>187</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>186</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>188</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>167</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>273</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>404</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>189</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>192</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>287</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>294</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>297</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>190</v>
       </c>
@@ -3744,28 +3744,28 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="17.25" customHeight="1">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="17.25" customHeight="1">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="17.25" customHeight="1">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="17.25" customHeight="1">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="20:23" ht="17.25" customHeight="1">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="20:23" ht="17.25" customHeight="1">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
+  <sortState ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3782,15 +3782,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90.75" thickBot="1">
       <c r="A2" s="15" t="s">
         <v>418</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3836,19 +3836,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -4507,41 +4507,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T28" sqref="T28"/>
+      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" customWidth="1"/>
+    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="15.75" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="29.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="29.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5307,7 +5307,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="29.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5636,9 +5636,6 @@
       </c>
       <c r="M22" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="X22" s="1" t="s">
         <v>84</v>
@@ -5648,7 +5645,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5690,7 +5687,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5736,7 +5733,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5778,7 +5775,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="15.75" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5829,7 +5826,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="15.75" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5883,7 +5880,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5924,7 +5921,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="15.75" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5966,7 +5963,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="15.75" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6013,7 +6010,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="15.75" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -6057,7 +6054,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -6114,7 +6111,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -6156,7 +6153,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -6246,7 +6243,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -6290,7 +6287,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -6343,7 +6340,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -6390,7 +6387,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6441,7 +6438,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="60">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6491,7 +6488,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6538,7 +6535,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="43.5">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6591,7 +6588,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6638,7 +6635,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6682,7 +6679,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6733,7 +6730,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6784,7 +6781,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6831,7 +6828,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6884,7 +6881,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="1" customFormat="1">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6931,7 +6928,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="1" customFormat="1">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6978,7 +6975,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -7029,7 +7026,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="1" customFormat="1">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -7076,7 +7073,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="1" customFormat="1">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -7129,7 +7126,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -7180,7 +7177,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="1" customFormat="1">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -7227,7 +7224,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="43.5">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -7284,7 +7281,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -7335,7 +7332,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -7382,7 +7379,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="43.5">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -7438,7 +7435,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7489,7 +7486,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="1" customFormat="1">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7536,7 +7533,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="1" customFormat="1">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7589,7 +7586,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7640,7 +7637,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="1" customFormat="1">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7687,7 +7684,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="1" customFormat="1">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7734,7 +7731,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="1" customFormat="1">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7781,7 +7778,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="1" customFormat="1">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7828,7 +7825,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7879,7 +7876,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="1" customFormat="1">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7932,7 +7929,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="1" customFormat="1">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7979,7 +7976,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="1" customFormat="1">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -8023,7 +8020,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -8074,7 +8071,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8127,7 +8124,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8174,7 +8171,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8227,7 +8224,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8274,7 +8271,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8327,7 +8324,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="1" customFormat="1">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8370,7 +8367,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="18">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8420,7 +8417,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="18">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8470,7 +8467,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="18">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8520,7 +8517,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="18">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8570,7 +8567,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="18">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8620,7 +8617,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="18">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8670,7 +8667,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="29.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8720,7 +8717,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="18">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8770,7 +8767,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="18">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8820,7 +8817,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="18">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8870,7 +8867,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8923,7 +8920,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8973,7 +8970,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -9026,7 +9023,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="38.1" customHeight="1">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -9082,12 +9079,12 @@
         <v>716</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
+  <sortState ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9107,21 +9104,21 @@
       <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="66" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -9153,7 +9150,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -9176,7 +9173,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -9199,7 +9196,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -9222,7 +9219,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -9245,7 +9242,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -9274,7 +9271,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9297,7 +9294,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -9320,7 +9317,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -9344,7 +9341,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9369,7 +9366,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -9393,7 +9390,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -9416,7 +9413,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9445,7 +9442,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9468,7 +9465,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9491,7 +9488,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9520,7 +9517,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9544,7 +9541,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9573,7 +9570,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9598,7 +9595,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9622,7 +9619,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9645,7 +9642,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9669,7 +9666,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9694,7 +9691,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9719,7 +9716,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9744,7 +9741,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9767,7 +9764,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9790,7 +9787,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9813,7 +9810,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9842,7 +9839,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9871,7 +9868,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9900,7 +9897,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9929,7 +9926,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9961,7 +9958,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9990,7 +9987,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -10019,7 +10016,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="1" customFormat="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -10048,7 +10045,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -10077,7 +10074,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="1" customFormat="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -10106,7 +10103,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="1" customFormat="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -10135,7 +10132,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="1" customFormat="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -10164,7 +10161,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -10196,7 +10193,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -10225,7 +10222,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -10257,7 +10254,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="1" customFormat="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -10286,7 +10283,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="1" customFormat="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -10315,7 +10312,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" s="1" customFormat="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -10344,7 +10341,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" s="1" customFormat="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -10373,7 +10370,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="1" customFormat="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -10402,7 +10399,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" s="1" customFormat="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -10431,7 +10428,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" s="1" customFormat="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -10460,7 +10457,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" s="1" customFormat="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -10489,7 +10486,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="1" customFormat="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -10518,7 +10515,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" s="1" customFormat="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10547,7 +10544,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" s="1" customFormat="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10576,7 +10573,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" s="1" customFormat="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10605,7 +10602,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" s="1" customFormat="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10634,7 +10631,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" s="1" customFormat="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10663,7 +10660,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" s="1" customFormat="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10692,7 +10689,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" s="1" customFormat="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10724,7 +10721,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" s="1" customFormat="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10756,7 +10753,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" s="1" customFormat="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10785,7 +10782,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" s="1" customFormat="1">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10817,7 +10814,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" s="1" customFormat="1">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -10846,7 +10843,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" s="1" customFormat="1">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -10875,7 +10872,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="1" customFormat="1">
       <c r="A65" s="1">
         <v>58</v>
       </c>
@@ -10907,7 +10904,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="1" customFormat="1">
       <c r="A66" s="1">
         <v>59</v>
       </c>
@@ -10939,7 +10936,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" s="1" customFormat="1">
       <c r="A67" s="1">
         <v>61</v>
       </c>
@@ -10971,7 +10968,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" s="1" customFormat="1">
       <c r="A68" s="1">
         <v>62</v>
       </c>
@@ -11003,7 +11000,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" s="1" customFormat="1">
       <c r="A69" s="1">
         <v>63</v>
       </c>
@@ -11035,7 +11032,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="15.75">
       <c r="A70" s="1">
         <v>64</v>
       </c>
@@ -11073,7 +11070,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="1" customFormat="1">
       <c r="A71" s="1">
         <v>58</v>
       </c>
@@ -11105,7 +11102,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="1" customFormat="1">
       <c r="A72" s="1">
         <v>59</v>
       </c>
@@ -11137,7 +11134,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="1" customFormat="1">
       <c r="A73" s="1">
         <v>60</v>
       </c>
@@ -11169,7 +11166,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="1" customFormat="1">
       <c r="A74" s="1">
         <v>61</v>
       </c>
@@ -11201,7 +11198,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="1" customFormat="1">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -11230,7 +11227,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="1" customFormat="1">
       <c r="A76" s="1">
         <v>39</v>
       </c>
@@ -11259,7 +11256,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="1" customFormat="1">
       <c r="A77" s="1">
         <v>43</v>
       </c>
@@ -11286,7 +11283,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="1" customFormat="1">
       <c r="A78" s="1">
         <v>40</v>
       </c>
@@ -11318,7 +11315,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
       <c r="A79" s="1">
         <v>42</v>
       </c>
@@ -11350,7 +11347,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" s="1" customFormat="1">
       <c r="A80" s="1">
         <v>41</v>
       </c>
@@ -11379,7 +11376,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" s="1" customFormat="1">
       <c r="A81" s="1">
         <v>43</v>
       </c>
@@ -11408,7 +11405,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" s="1" customFormat="1">
       <c r="A82" s="1">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
add Prov, Pulse Ox and remove Medstatement from Cap Statements
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE6E690-5639-4785-BC70-DC2A5273A894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3498B64A-2956-49F1-B39F-94612D545383}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="resources" sheetId="4" r:id="rId4"/>
     <sheet name="ops" sheetId="5" r:id="rId5"/>
     <sheet name="interactions" sheetId="6" r:id="rId6"/>
-    <sheet name="sps" sheetId="7" r:id="rId7"/>
-    <sheet name="sp_combos" sheetId="8" r:id="rId8"/>
+    <sheet name="rest_interactions" sheetId="11" r:id="rId7"/>
+    <sheet name="sps" sheetId="7" r:id="rId8"/>
+    <sheet name="sp_combos" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sp_combos!$B$1:$B$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">sps!$A$1:$AB$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sp_combos!$B$1:$B$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sps!$A$1:$AB$92</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -38,6 +39,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{5BD04D3A-61B4-4353-A042-87021061D1BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>User</author>
@@ -71,7 +106,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>User</author>
@@ -106,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="801">
   <si>
     <t>Element</t>
   </si>
@@ -1512,9 +1547,6 @@
   </si>
   <si>
     <t>US Core Laboratory Result Observation Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.r4-4.0.0</t>
   </si>
   <si>
     <t>shall_modifier</t>
@@ -2476,6 +2508,51 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-device</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>search-system</t>
+  </si>
+  <si>
+    <t>history-system</t>
+  </si>
+  <si>
+    <t>The MedicationRequest resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+ For example, A server **SHALL** be capable of returning all medications for a patient using one of or both:
+ `GET /MedicationRequest?patient=[id]`
+ `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.argo-3.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-pulse-oximetry</t>
+  </si>
+  <si>
+    <t>US Core Pulse Oximetry Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-provenance</t>
+  </si>
+  <si>
+    <t>US Core Provenance Profile</t>
+  </si>
+  <si>
+    <t>Provenance</t>
+  </si>
+  <si>
+    <t>conf_Provenance</t>
+  </si>
+  <si>
+    <t>Provenance:target</t>
   </si>
 </sst>
 </file>
@@ -2944,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2982,8 +3059,8 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>468</v>
+      <c r="B4" s="11" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3039,11 +3116,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3103,7 +3180,7 @@
         <v>385</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>73</v>
@@ -3250,10 +3327,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>779</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>73</v>
@@ -3385,10 +3462,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>781</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>73</v>
@@ -3398,39 +3475,66 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:6" s="1" customFormat="1">
+      <c r="A24" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="1" customFormat="1">
+      <c r="A25" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:6" s="1" customFormat="1">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="1"/>
+    </row>
+    <row r="27" spans="1:6" s="1" customFormat="1">
+      <c r="A27" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>798</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3438,11 +3542,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
@@ -3545,6 +3649,9 @@
       <c r="D2"/>
       <c r="F2"/>
       <c r="R2"/>
+      <c r="W2" s="1" t="s">
+        <v>800</v>
+      </c>
       <c r="X2" t="s">
         <v>20</v>
       </c>
@@ -3556,6 +3663,9 @@
       <c r="B3" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W3" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="4" spans="1:24" ht="17.25" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -3564,6 +3674,9 @@
       <c r="B4" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W4" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="17.25" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -3572,6 +3685,9 @@
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W5" s="1" t="s">
+        <v>800</v>
+      </c>
       <c r="X5" t="s">
         <v>24</v>
       </c>
@@ -3583,6 +3699,9 @@
       <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W6" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -3591,6 +3710,9 @@
       <c r="B7" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W7" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -3602,6 +3724,9 @@
       <c r="C8" s="2" t="s">
         <v>464</v>
       </c>
+      <c r="W8" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -3610,6 +3735,9 @@
       <c r="B9" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W9" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -3618,6 +3746,9 @@
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W10" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -3626,6 +3757,9 @@
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W11" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -3634,6 +3768,9 @@
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="W12" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -3645,6 +3782,9 @@
       <c r="C13" s="2" t="s">
         <v>451</v>
       </c>
+      <c r="W13" s="1" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -3654,10 +3794,13 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>785</v>
+        <v>792</v>
       </c>
       <c r="U14" s="7" t="s">
         <v>219</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
@@ -3668,10 +3811,13 @@
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>448</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17.25" customHeight="1">
@@ -3681,32 +3827,44 @@
       <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W16" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W17" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W18" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>294</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W19" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>297</v>
       </c>
@@ -3716,25 +3874,37 @@
       <c r="U20" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W20" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="17.25" customHeight="1">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:21" ht="17.25" customHeight="1">
+      <c r="W21" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="1" customFormat="1" ht="15">
+      <c r="A22" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:23" ht="17.25" customHeight="1">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21" ht="17.25" customHeight="1">
+    <row r="24" spans="1:23" ht="17.25" customHeight="1">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21" ht="17.25" customHeight="1">
+    <row r="25" spans="1:23" ht="17.25" customHeight="1">
       <c r="A25"/>
     </row>
     <row r="56" spans="20:23" ht="17.25" customHeight="1">
@@ -3802,7 +3972,7 @@
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3815,10 +3985,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3827,9 +3997,10 @@
     <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3849,7 +4020,7 @@
         <v>422</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>423</v>
@@ -3896,8 +4067,11 @@
       <c r="V1" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="W1" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3917,7 +4091,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -3964,8 +4138,11 @@
       <c r="V2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -4029,8 +4206,11 @@
       <c r="V3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="W3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -4094,8 +4274,11 @@
       <c r="V4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="W4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -4159,8 +4342,11 @@
       <c r="V5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="W5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -4225,8 +4411,11 @@
       <c r="V6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="W6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -4290,8 +4479,11 @@
       <c r="V7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="W7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -4355,8 +4547,11 @@
       <c r="V8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:22">
+      <c r="W8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -4420,8 +4615,11 @@
       <c r="V9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="W9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -4483,6 +4681,9 @@
         <v>32</v>
       </c>
       <c r="V10" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4492,14 +4693,76 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B34E79-4E3A-4FF0-901F-87AE2E2F7A43}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="AA42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4573,19 +4836,19 @@
         <v>48</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>50</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>51</v>
@@ -4645,7 +4908,7 @@
         <v>58</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>57</v>
@@ -4660,7 +4923,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="1" customFormat="1">
@@ -4693,7 +4956,7 @@
         <v>58</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>57</v>
@@ -4705,7 +4968,7 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="12"/>
       <c r="AB3" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -4738,7 +5001,7 @@
         <v>83</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>57</v>
@@ -4757,7 +5020,7 @@
       </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" spans="1:28" s="1" customFormat="1" ht="29.25">
@@ -4790,7 +5053,7 @@
         <v>95</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>57</v>
@@ -4802,16 +5065,16 @@
         <v>96</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="Z5" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="AA5" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AB5" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:28" s="1" customFormat="1">
@@ -4844,7 +5107,7 @@
         <v>58</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>57</v>
@@ -4859,7 +5122,7 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="12"/>
       <c r="AB6" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
@@ -4892,7 +5155,7 @@
         <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K7" t="s">
         <v>57</v>
@@ -4908,7 +5171,7 @@
       </c>
       <c r="AA7" s="12"/>
       <c r="AB7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -4941,7 +5204,7 @@
         <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>57</v>
@@ -4957,7 +5220,7 @@
       </c>
       <c r="AA8" s="12"/>
       <c r="AB8" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -4990,7 +5253,7 @@
         <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>57</v>
@@ -5002,7 +5265,7 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="12"/>
       <c r="AB9" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="29.25">
@@ -5035,7 +5298,7 @@
         <v>95</v>
       </c>
       <c r="J10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>57</v>
@@ -5052,13 +5315,13 @@
         <v>77</v>
       </c>
       <c r="Z10" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="AA10" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="AA10" s="12" t="s">
+      <c r="AB10" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -5091,7 +5354,7 @@
         <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>57</v>
@@ -5107,7 +5370,7 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="12"/>
       <c r="AB11" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -5140,7 +5403,7 @@
         <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>57</v>
@@ -5153,7 +5416,7 @@
       </c>
       <c r="AA12" s="12"/>
       <c r="AB12" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -5186,7 +5449,7 @@
         <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>57</v>
@@ -5201,13 +5464,13 @@
         <v>147</v>
       </c>
       <c r="Z13" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="AA13" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="AA13" s="12" t="s">
+      <c r="AB13" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1">
@@ -5240,7 +5503,7 @@
         <v>58</v>
       </c>
       <c r="J14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>57</v>
@@ -5258,7 +5521,7 @@
         <v>178</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -5291,7 +5554,7 @@
         <v>58</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>57</v>
@@ -5306,7 +5569,7 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1">
@@ -5339,7 +5602,7 @@
         <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>57</v>
@@ -5358,7 +5621,7 @@
       </c>
       <c r="AA16" s="12"/>
       <c r="AB16" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="29.25">
@@ -5391,7 +5654,7 @@
         <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>57</v>
@@ -5406,10 +5669,10 @@
         <v>166</v>
       </c>
       <c r="AA17" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB17" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -5442,7 +5705,7 @@
         <v>95</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>57</v>
@@ -5457,13 +5720,13 @@
         <v>97</v>
       </c>
       <c r="Z18" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="AA18" s="12" t="s">
         <v>513</v>
       </c>
-      <c r="AA18" s="12" t="s">
+      <c r="AB18" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -5496,7 +5759,7 @@
         <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>57</v>
@@ -5511,7 +5774,7 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="12"/>
       <c r="AB19" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:28">
@@ -5544,7 +5807,7 @@
         <v>58</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>57</v>
@@ -5557,7 +5820,7 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="12"/>
       <c r="AB20" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="21" spans="1:28">
@@ -5590,7 +5853,7 @@
         <v>58</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>57</v>
@@ -5605,7 +5868,7 @@
         <v>374</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="22" spans="1:28">
@@ -5638,7 +5901,7 @@
         <v>83</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>57</v>
@@ -5651,7 +5914,7 @@
       </c>
       <c r="Z22"/>
       <c r="AB22" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -5694,7 +5957,7 @@
       </c>
       <c r="Y23"/>
       <c r="AB23" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="24" spans="1:28">
@@ -5727,7 +5990,7 @@
         <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>57</v>
@@ -5741,7 +6004,7 @@
       <c r="Y24"/>
       <c r="AA24" s="12"/>
       <c r="AB24" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1">
@@ -5784,7 +6047,7 @@
       </c>
       <c r="AA25" s="12"/>
       <c r="AB25" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1">
@@ -5817,7 +6080,7 @@
         <v>58</v>
       </c>
       <c r="J26" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>57</v>
@@ -5833,10 +6096,10 @@
         <v>165</v>
       </c>
       <c r="AA26" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="AB26" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="AB26" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1">
@@ -5869,7 +6132,7 @@
         <v>66</v>
       </c>
       <c r="J27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>57</v>
@@ -5888,10 +6151,10 @@
         <v>181</v>
       </c>
       <c r="AA27" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AB27" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="AB27" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -5933,7 +6196,7 @@
         <v>57</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1">
@@ -5966,7 +6229,7 @@
         <v>75</v>
       </c>
       <c r="J29" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>57</v>
@@ -5976,7 +6239,7 @@
       </c>
       <c r="X29"/>
       <c r="AB29" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1">
@@ -6009,7 +6272,7 @@
         <v>66</v>
       </c>
       <c r="J30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>57</v>
@@ -6024,7 +6287,7 @@
         <v>72</v>
       </c>
       <c r="AB30" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1">
@@ -6057,7 +6320,7 @@
         <v>58</v>
       </c>
       <c r="J31" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>57</v>
@@ -6069,7 +6332,7 @@
         <v>64</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6102,7 +6365,7 @@
         <v>66</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>57</v>
@@ -6127,7 +6390,7 @@
       </c>
       <c r="AA32" s="2"/>
       <c r="AB32" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6160,7 +6423,7 @@
         <v>62</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>57</v>
@@ -6170,7 +6433,7 @@
       </c>
       <c r="AA33" s="2"/>
       <c r="AB33" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6203,7 +6466,7 @@
         <v>58</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>57</v>
@@ -6213,7 +6476,7 @@
       </c>
       <c r="AA34" s="2"/>
       <c r="AB34" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6246,7 +6509,7 @@
         <v>83</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>57</v>
@@ -6262,7 +6525,7 @@
       </c>
       <c r="AA35" s="12"/>
       <c r="AB35" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="36" spans="1:28" s="1" customFormat="1">
@@ -6295,7 +6558,7 @@
         <v>58</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>57</v>
@@ -6307,7 +6570,7 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="12"/>
       <c r="AB36" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="37" spans="1:28" s="1" customFormat="1">
@@ -6340,7 +6603,7 @@
         <v>95</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>57</v>
@@ -6352,16 +6615,16 @@
         <v>96</v>
       </c>
       <c r="Y37" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="Z37" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="Z37" s="5" t="s">
+      <c r="AA37" s="12" t="s">
         <v>554</v>
       </c>
-      <c r="AA37" s="12" t="s">
+      <c r="AB37" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="AB37" s="1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:28" s="1" customFormat="1">
@@ -6394,7 +6657,7 @@
         <v>58</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>57</v>
@@ -6409,7 +6672,7 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="12"/>
       <c r="AB38" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6442,7 +6705,7 @@
         <v>83</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>57</v>
@@ -6461,7 +6724,7 @@
       </c>
       <c r="AA39" s="12"/>
       <c r="AB39" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="40" spans="1:28" s="1" customFormat="1" ht="60">
@@ -6494,7 +6757,7 @@
         <v>58</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>57</v>
@@ -6512,7 +6775,7 @@
         <v>320</v>
       </c>
       <c r="AB40" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="41" spans="1:28" s="1" customFormat="1">
@@ -6545,7 +6808,7 @@
         <v>58</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>57</v>
@@ -6560,7 +6823,7 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="12"/>
       <c r="AB41" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="42" spans="1:28" s="1" customFormat="1" ht="43.5">
@@ -6593,7 +6856,7 @@
         <v>95</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>57</v>
@@ -6605,16 +6868,16 @@
         <v>96</v>
       </c>
       <c r="Y42" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="Z42" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="Z42" s="5" t="s">
+      <c r="AA42" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="AA42" s="12" t="s">
+      <c r="AB42" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="AB42" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="43" spans="1:28" s="1" customFormat="1">
@@ -6647,7 +6910,7 @@
         <v>58</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>57</v>
@@ -6662,7 +6925,7 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="12"/>
       <c r="AB43" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:28" s="1" customFormat="1">
@@ -6695,7 +6958,7 @@
         <v>58</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>57</v>
@@ -6707,7 +6970,7 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="12"/>
       <c r="AB44" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6740,7 +7003,7 @@
         <v>83</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>57</v>
@@ -6759,7 +7022,7 @@
       </c>
       <c r="AA45" s="12"/>
       <c r="AB45" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -6811,7 +7074,7 @@
       </c>
       <c r="AA46" s="12"/>
       <c r="AB46" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="47" spans="1:28" s="1" customFormat="1">
@@ -6844,7 +7107,7 @@
         <v>58</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>57</v>
@@ -6859,7 +7122,7 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="12"/>
       <c r="AB47" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="48" spans="1:28" s="1" customFormat="1">
@@ -6892,7 +7155,7 @@
         <v>95</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>57</v>
@@ -6904,16 +7167,16 @@
         <v>96</v>
       </c>
       <c r="Y48" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="Z48" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="Z48" s="5" t="s">
+      <c r="AA48" s="12" t="s">
         <v>581</v>
       </c>
-      <c r="AA48" s="12" t="s">
+      <c r="AB48" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="AB48" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="49" spans="1:28" s="1" customFormat="1">
@@ -6946,7 +7209,7 @@
         <v>58</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>57</v>
@@ -6961,7 +7224,7 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="12"/>
       <c r="AB49" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="50" spans="1:28" s="1" customFormat="1">
@@ -6994,7 +7257,7 @@
         <v>58</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>57</v>
@@ -7009,7 +7272,7 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="12"/>
       <c r="AB50" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7042,7 +7305,7 @@
         <v>83</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>57</v>
@@ -7061,7 +7324,7 @@
       </c>
       <c r="AA51" s="12"/>
       <c r="AB51" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="52" spans="1:28" s="1" customFormat="1">
@@ -7094,7 +7357,7 @@
         <v>58</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>57</v>
@@ -7109,7 +7372,7 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="12"/>
       <c r="AB52" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="53" spans="1:28" s="1" customFormat="1">
@@ -7142,7 +7405,7 @@
         <v>95</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>57</v>
@@ -7154,16 +7417,16 @@
         <v>96</v>
       </c>
       <c r="Y53" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="Z53" s="5" t="s">
         <v>593</v>
       </c>
-      <c r="Z53" s="5" t="s">
+      <c r="AA53" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="AA53" s="12" t="s">
+      <c r="AB53" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="AB53" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7174,7 +7437,7 @@
         <v>188</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>32</v>
@@ -7196,7 +7459,7 @@
         <v>83</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>57</v>
@@ -7215,7 +7478,7 @@
       </c>
       <c r="AA54" s="12"/>
       <c r="AB54" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="55" spans="1:28" s="1" customFormat="1">
@@ -7248,7 +7511,7 @@
         <v>58</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>57</v>
@@ -7263,7 +7526,7 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="12"/>
       <c r="AB55" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="56" spans="1:28" s="1" customFormat="1" ht="43.5">
@@ -7296,7 +7559,7 @@
         <v>95</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>57</v>
@@ -7318,10 +7581,10 @@
         <v>376</v>
       </c>
       <c r="AA56" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="AB56" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="AB56" s="1" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7354,7 +7617,7 @@
         <v>83</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>57</v>
@@ -7373,7 +7636,7 @@
       </c>
       <c r="AA57" s="12"/>
       <c r="AB57" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="58" spans="1:28" s="1" customFormat="1">
@@ -7406,7 +7669,7 @@
         <v>58</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>57</v>
@@ -7421,7 +7684,7 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="12"/>
       <c r="AB58" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="59" spans="1:28" s="1" customFormat="1" ht="43.5">
@@ -7454,7 +7717,7 @@
         <v>95</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>57</v>
@@ -7475,10 +7738,10 @@
         <v>377</v>
       </c>
       <c r="AA59" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="AB59" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="AB59" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7511,7 +7774,7 @@
         <v>83</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>57</v>
@@ -7530,7 +7793,7 @@
       </c>
       <c r="AA60" s="12"/>
       <c r="AB60" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="61" spans="1:28" s="1" customFormat="1">
@@ -7563,7 +7826,7 @@
         <v>58</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>57</v>
@@ -7578,7 +7841,7 @@
       <c r="Z61" s="5"/>
       <c r="AA61" s="12"/>
       <c r="AB61" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="62" spans="1:28" s="1" customFormat="1">
@@ -7611,7 +7874,7 @@
         <v>95</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>57</v>
@@ -7623,16 +7886,16 @@
         <v>96</v>
       </c>
       <c r="Y62" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="Z62" s="5" t="s">
         <v>227</v>
       </c>
       <c r="AA62" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="AB62" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="AB62" s="1" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7665,7 +7928,7 @@
         <v>83</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>57</v>
@@ -7684,7 +7947,7 @@
       </c>
       <c r="AA63" s="12"/>
       <c r="AB63" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="64" spans="1:28" s="1" customFormat="1">
@@ -7717,7 +7980,7 @@
         <v>58</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>57</v>
@@ -7732,7 +7995,7 @@
       <c r="Z64" s="5"/>
       <c r="AA64" s="12"/>
       <c r="AB64" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="65" spans="1:28" s="1" customFormat="1">
@@ -7765,7 +8028,7 @@
         <v>58</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>57</v>
@@ -7780,7 +8043,7 @@
       <c r="Z65" s="5"/>
       <c r="AA65" s="12"/>
       <c r="AB65" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="66" spans="1:28" s="1" customFormat="1">
@@ -7813,7 +8076,7 @@
         <v>58</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>57</v>
@@ -7828,7 +8091,7 @@
       <c r="Z66" s="5"/>
       <c r="AA66" s="12"/>
       <c r="AB66" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="67" spans="1:28" s="1" customFormat="1">
@@ -7861,7 +8124,7 @@
         <v>58</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>57</v>
@@ -7876,7 +8139,7 @@
       <c r="Z67" s="5"/>
       <c r="AA67" s="12"/>
       <c r="AB67" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -7909,7 +8172,7 @@
         <v>83</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>57</v>
@@ -7928,7 +8191,7 @@
       </c>
       <c r="AA68" s="12"/>
       <c r="AB68" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="69" spans="1:28" s="1" customFormat="1">
@@ -7961,7 +8224,7 @@
         <v>95</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>57</v>
@@ -7973,16 +8236,16 @@
         <v>96</v>
       </c>
       <c r="Y69" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="Z69" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="Z69" s="5" t="s">
+      <c r="AA69" s="12" t="s">
         <v>634</v>
       </c>
-      <c r="AA69" s="12" t="s">
+      <c r="AB69" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="AB69" s="1" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="70" spans="1:28" s="1" customFormat="1">
@@ -8015,7 +8278,7 @@
         <v>58</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>57</v>
@@ -8030,7 +8293,7 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="12"/>
       <c r="AB70" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="71" spans="1:28" s="1" customFormat="1">
@@ -8063,7 +8326,7 @@
         <v>58</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>57</v>
@@ -8075,7 +8338,7 @@
       <c r="Z71" s="5"/>
       <c r="AA71" s="12"/>
       <c r="AB71" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -8108,7 +8371,7 @@
         <v>83</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>57</v>
@@ -8127,7 +8390,7 @@
       </c>
       <c r="AA72" s="12"/>
       <c r="AB72" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="73" spans="1:28" s="1" customFormat="1">
@@ -8160,7 +8423,7 @@
         <v>95</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>57</v>
@@ -8172,16 +8435,16 @@
         <v>96</v>
       </c>
       <c r="Y73" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="Z73" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="Z73" s="5" t="s">
+      <c r="AA73" s="12" t="s">
         <v>645</v>
       </c>
-      <c r="AA73" s="12" t="s">
+      <c r="AB73" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="AB73" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="74" spans="1:28" s="1" customFormat="1">
@@ -8214,7 +8477,7 @@
         <v>58</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>57</v>
@@ -8229,7 +8492,7 @@
       <c r="Z74" s="5"/>
       <c r="AA74" s="12"/>
       <c r="AB74" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="75" spans="1:28" s="1" customFormat="1">
@@ -8262,7 +8525,7 @@
         <v>95</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>57</v>
@@ -8274,16 +8537,16 @@
         <v>96</v>
       </c>
       <c r="Y75" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="Z75" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="Z75" s="5" t="s">
+      <c r="AA75" s="12" t="s">
         <v>652</v>
       </c>
-      <c r="AA75" s="12" t="s">
+      <c r="AB75" s="1" t="s">
         <v>653</v>
-      </c>
-      <c r="AB75" s="1" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="76" spans="1:28" s="1" customFormat="1">
@@ -8316,7 +8579,7 @@
         <v>58</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>57</v>
@@ -8331,7 +8594,7 @@
       <c r="Z76" s="5"/>
       <c r="AA76" s="12"/>
       <c r="AB76" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="77" spans="1:28" s="1" customFormat="1">
@@ -8364,7 +8627,7 @@
         <v>95</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>57</v>
@@ -8376,16 +8639,16 @@
         <v>96</v>
       </c>
       <c r="Y77" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="Z77" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="Z77" s="5" t="s">
+      <c r="AA77" s="12" t="s">
         <v>659</v>
       </c>
-      <c r="AA77" s="12" t="s">
+      <c r="AB77" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="AB77" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="78" spans="1:28" s="1" customFormat="1">
@@ -8418,7 +8681,7 @@
         <v>58</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>57</v>
@@ -8429,7 +8692,7 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
       <c r="AB78" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="18">
@@ -8462,7 +8725,7 @@
         <v>66</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>57</v>
@@ -8477,10 +8740,10 @@
         <v>282</v>
       </c>
       <c r="AA79" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="AB79" t="s">
         <v>665</v>
-      </c>
-      <c r="AB79" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="18">
@@ -8513,7 +8776,7 @@
         <v>66</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>57</v>
@@ -8528,10 +8791,10 @@
         <v>283</v>
       </c>
       <c r="AA80" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="AB80" t="s">
         <v>668</v>
-      </c>
-      <c r="AB80" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="81" spans="1:28" ht="18">
@@ -8564,7 +8827,7 @@
         <v>66</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>57</v>
@@ -8579,10 +8842,10 @@
         <v>286</v>
       </c>
       <c r="AA81" s="12" t="s">
+        <v>670</v>
+      </c>
+      <c r="AB81" t="s">
         <v>671</v>
-      </c>
-      <c r="AB81" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="82" spans="1:28" ht="18">
@@ -8615,7 +8878,7 @@
         <v>66</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>57</v>
@@ -8630,10 +8893,10 @@
         <v>285</v>
       </c>
       <c r="AA82" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="AB82" t="s">
         <v>674</v>
-      </c>
-      <c r="AB82" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="83" spans="1:28" ht="18">
@@ -8666,7 +8929,7 @@
         <v>66</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>57</v>
@@ -8681,10 +8944,10 @@
         <v>284</v>
       </c>
       <c r="AA83" s="12" t="s">
+        <v>676</v>
+      </c>
+      <c r="AB83" t="s">
         <v>677</v>
-      </c>
-      <c r="AB83" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="84" spans="1:28" s="1" customFormat="1" ht="18">
@@ -8717,7 +8980,7 @@
         <v>66</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>57</v>
@@ -8732,10 +8995,10 @@
         <v>282</v>
       </c>
       <c r="AA84" s="12" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB84" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="AB84" s="1" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="85" spans="1:28" s="1" customFormat="1" ht="29.25">
@@ -8768,7 +9031,7 @@
         <v>66</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>57</v>
@@ -8783,10 +9046,10 @@
         <v>283</v>
       </c>
       <c r="AA85" s="12" t="s">
+        <v>682</v>
+      </c>
+      <c r="AB85" s="1" t="s">
         <v>683</v>
-      </c>
-      <c r="AB85" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="86" spans="1:28" s="1" customFormat="1" ht="18">
@@ -8819,7 +9082,7 @@
         <v>66</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>57</v>
@@ -8834,10 +9097,10 @@
         <v>286</v>
       </c>
       <c r="AA86" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="AB86" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="AB86" s="1" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="87" spans="1:28" s="1" customFormat="1" ht="18">
@@ -8870,7 +9133,7 @@
         <v>66</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>57</v>
@@ -8885,10 +9148,10 @@
         <v>285</v>
       </c>
       <c r="AA87" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="AB87" s="1" t="s">
         <v>689</v>
-      </c>
-      <c r="AB87" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="88" spans="1:28" s="1" customFormat="1" ht="18">
@@ -8921,7 +9184,7 @@
         <v>66</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>57</v>
@@ -8936,10 +9199,10 @@
         <v>284</v>
       </c>
       <c r="AA88" s="12" t="s">
+        <v>691</v>
+      </c>
+      <c r="AB88" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="AB88" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -8972,7 +9235,7 @@
         <v>66</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>57</v>
@@ -8990,10 +9253,10 @@
         <v>296</v>
       </c>
       <c r="AA89" s="12" t="s">
+        <v>694</v>
+      </c>
+      <c r="AB89" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="AB89" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -9026,7 +9289,7 @@
         <v>58</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>57</v>
@@ -9041,10 +9304,10 @@
         <v>380</v>
       </c>
       <c r="AA90" s="12" t="s">
+        <v>697</v>
+      </c>
+      <c r="AB90" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="AB90" s="1" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
@@ -9077,7 +9340,7 @@
         <v>58</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>57</v>
@@ -9095,10 +9358,10 @@
         <v>379</v>
       </c>
       <c r="AA91" s="12" t="s">
+        <v>700</v>
+      </c>
+      <c r="AB91" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="AB91" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="92" spans="1:28" ht="38.1" customHeight="1">
@@ -9131,7 +9394,7 @@
         <v>95</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>57</v>
@@ -9152,10 +9415,10 @@
         <v>378</v>
       </c>
       <c r="AA92" s="12" t="s">
+        <v>703</v>
+      </c>
+      <c r="AB92" t="s">
         <v>704</v>
-      </c>
-      <c r="AB92" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="93" spans="1:28">
@@ -9172,7 +9435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
@@ -9237,7 +9500,7 @@
         <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D2" t="s">
         <v>104</v>
@@ -9249,7 +9512,7 @@
         <v>105</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -9260,7 +9523,7 @@
         <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D3" t="s">
         <v>106</v>
@@ -9272,7 +9535,7 @@
         <v>107</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -9283,7 +9546,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>
@@ -9295,7 +9558,7 @@
         <v>107</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -9306,7 +9569,7 @@
         <v>163</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D5" t="s">
         <v>109</v>
@@ -9318,7 +9581,7 @@
         <v>105</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -9347,7 +9610,7 @@
         <v>341</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -9358,7 +9621,7 @@
         <v>163</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D7" t="s">
         <v>112</v>
@@ -9370,7 +9633,7 @@
         <v>111</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -9381,7 +9644,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D8" t="s">
         <v>113</v>
@@ -9393,7 +9656,7 @@
         <v>111</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -9404,7 +9667,7 @@
         <v>163</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D9" t="s">
         <v>114</v>
@@ -9417,7 +9680,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -9428,7 +9691,7 @@
         <v>163</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D10" t="s">
         <v>115</v>
@@ -9442,7 +9705,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -9453,7 +9716,7 @@
         <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D11" t="s">
         <v>116</v>
@@ -9466,7 +9729,7 @@
       </c>
       <c r="H11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -9477,7 +9740,7 @@
         <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D12" t="s">
         <v>99</v>
@@ -9489,7 +9752,7 @@
         <v>58</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -9518,7 +9781,7 @@
         <v>342</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -9529,7 +9792,7 @@
         <v>163</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D14" t="s">
         <v>119</v>
@@ -9541,7 +9804,7 @@
         <v>107</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -9552,7 +9815,7 @@
         <v>163</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D15" t="s">
         <v>120</v>
@@ -9564,7 +9827,7 @@
         <v>105</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -9593,7 +9856,7 @@
         <v>343</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -9604,7 +9867,7 @@
         <v>163</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D17" t="s">
         <v>122</v>
@@ -9617,7 +9880,7 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -9646,7 +9909,7 @@
         <v>344</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -9657,7 +9920,7 @@
         <v>163</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -9671,7 +9934,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -9682,7 +9945,7 @@
         <v>164</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D20" t="s">
         <v>125</v>
@@ -9695,7 +9958,7 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -9706,7 +9969,7 @@
         <v>164</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D21" t="s">
         <v>127</v>
@@ -9718,7 +9981,7 @@
         <v>128</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -9729,7 +9992,7 @@
         <v>164</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D22" t="s">
         <v>129</v>
@@ -9742,7 +10005,7 @@
       </c>
       <c r="H22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -9753,7 +10016,7 @@
         <v>164</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D23" t="s">
         <v>131</v>
@@ -9767,7 +10030,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -9778,7 +10041,7 @@
         <v>164</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D24" t="s">
         <v>133</v>
@@ -9792,7 +10055,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -9803,7 +10066,7 @@
         <v>164</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D25" t="s">
         <v>134</v>
@@ -9817,7 +10080,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -9828,7 +10091,7 @@
         <v>164</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D26" t="s">
         <v>135</v>
@@ -9840,7 +10103,7 @@
         <v>132</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -9851,7 +10114,7 @@
         <v>164</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D27" t="s">
         <v>136</v>
@@ -9863,7 +10126,7 @@
         <v>58</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -9874,7 +10137,7 @@
         <v>164</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D28" t="s">
         <v>137</v>
@@ -9886,7 +10149,7 @@
         <v>132</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -9915,7 +10178,7 @@
         <v>185</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -9944,7 +10207,7 @@
         <v>182</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -9973,7 +10236,7 @@
         <v>184</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -10002,7 +10265,7 @@
         <v>183</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -10025,7 +10288,7 @@
         <v>111</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>161</v>
@@ -10179,7 +10442,7 @@
         <v>170</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="1" customFormat="1">
@@ -10208,7 +10471,7 @@
         <v>169</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="1" customFormat="1">
@@ -10237,7 +10500,7 @@
         <v>193</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
@@ -10269,7 +10532,7 @@
         <v>205</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
@@ -10298,7 +10561,7 @@
         <v>207</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
@@ -10330,7 +10593,7 @@
         <v>206</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="1" customFormat="1">
@@ -10359,7 +10622,7 @@
         <v>235</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="45" spans="1:10" s="1" customFormat="1">
@@ -10388,7 +10651,7 @@
         <v>193</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="1" customFormat="1">
@@ -10417,7 +10680,7 @@
         <v>212</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="1" customFormat="1">
@@ -10446,7 +10709,7 @@
         <v>207</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="1" customFormat="1">
@@ -10475,7 +10738,7 @@
         <v>213</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="1" customFormat="1">
@@ -10504,7 +10767,7 @@
         <v>235</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="1" customFormat="1">
@@ -10533,7 +10796,7 @@
         <v>352</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="1" customFormat="1">
@@ -10547,7 +10810,7 @@
         <v>409</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>73</v>
@@ -10559,10 +10822,10 @@
         <v>218</v>
       </c>
       <c r="I51" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>750</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="1" customFormat="1">
@@ -10588,7 +10851,7 @@
         <v>194</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J52" s="5" t="s">
         <v>251</v>
@@ -10617,7 +10880,7 @@
         <v>247</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>252</v>
@@ -10646,10 +10909,10 @@
         <v>196</v>
       </c>
       <c r="I54" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>754</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="1" customFormat="1">
@@ -10675,7 +10938,7 @@
         <v>248</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>253</v>
@@ -10707,7 +10970,7 @@
         <v>214</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="1" customFormat="1">
@@ -10736,7 +10999,7 @@
         <v>229</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="1" customFormat="1">
@@ -10765,7 +11028,7 @@
         <v>244</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="1" customFormat="1">
@@ -10829,7 +11092,7 @@
         <v>231</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="1" customFormat="1">
@@ -10858,7 +11121,7 @@
         <v>371</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="1" customFormat="1">
@@ -10890,7 +11153,7 @@
         <v>232</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="1" customFormat="1">
@@ -10919,7 +11182,7 @@
         <v>237</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="1" customFormat="1">
@@ -10948,7 +11211,7 @@
         <v>216</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="1" customFormat="1">
@@ -10980,7 +11243,7 @@
         <v>263</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="66" spans="1:16" s="1" customFormat="1">
@@ -11009,7 +11272,7 @@
         <v>261</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>265</v>
@@ -11073,7 +11336,7 @@
         <v>260</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>267</v>
@@ -11140,7 +11403,7 @@
         <v>304</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -11178,7 +11441,7 @@
         <v>311</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="72" spans="1:16" s="1" customFormat="1">
@@ -11210,7 +11473,7 @@
         <v>310</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="73" spans="1:16" s="1" customFormat="1">
@@ -11242,7 +11505,7 @@
         <v>313</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="74" spans="1:16" s="1" customFormat="1">
@@ -11274,7 +11537,7 @@
         <v>315</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="75" spans="1:16" s="1" customFormat="1">
@@ -11303,7 +11566,7 @@
         <v>314</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="1" customFormat="1">
@@ -11332,7 +11595,7 @@
         <v>326</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="1" customFormat="1">
@@ -11343,7 +11606,7 @@
         <v>323</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>322</v>
@@ -11359,7 +11622,7 @@
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="78" spans="1:16" s="1" customFormat="1">
@@ -11481,7 +11744,7 @@
         <v>440</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="1" customFormat="1">
@@ -11492,7 +11755,7 @@
         <v>272</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
add $ expand to capstatements, fix qa error on endpoint example
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Argo-R4\source\source_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386B163F-A7D5-4AA1-90FA-8F13D22CF912}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3637578-0EF5-4001-8613-C0B94EB1E10B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="2715" windowWidth="18900" windowHeight="11055" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22815" yWindow="-75" windowWidth="21510" windowHeight="14085" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="531">
   <si>
     <t>Element</t>
   </si>
@@ -1599,9 +1599,6 @@
  `GET /MedicationRequest?patient=[id]&amp;_include=MedicationRequest:medication`</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core.argo-3.1.0</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-pulse-oximetry</t>
   </si>
   <si>
@@ -1729,6 +1726,24 @@
   </si>
   <si>
     <t>Fetches an AllergyIntolerance resource  (within the clients authorization scope) and any corresponding Provenance resources.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core-3.0.1</t>
+  </si>
+  <si>
+    <t>ValueSet</t>
+  </si>
+  <si>
+    <t>A  client can determine the note and report types support by a server by invoking the standard FHIR Value Set Expansion ($expand) operation defined in the FHIR R4 specification. Because servers may support different read and write formats, it also is used to determine the formats (for example, text, pdf) the server supports read and write transactions.</t>
+  </si>
+  <si>
+    <t>expand</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/OperationDefinition/ValueSet-expand</t>
+  </si>
+  <si>
+    <t>conf_ValueSet</t>
   </si>
 </sst>
 </file>
@@ -2212,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2251,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>482</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2288,7 +2303,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2310,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2668,10 +2683,10 @@
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>484</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -2710,16 +2725,16 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -2734,10 +2749,10 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T16" sqref="T16"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
@@ -2957,7 +2972,7 @@
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
@@ -3022,15 +3037,21 @@
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1" ht="15">
       <c r="A22" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="17.25" customHeight="1">
-      <c r="A23"/>
+    <row r="23" spans="1:21" s="1" customFormat="1" ht="15">
+      <c r="A23" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:21" ht="17.25" customHeight="1">
       <c r="A24"/>
@@ -3061,7 +3082,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3106,6 +3127,23 @@
         <v>470</v>
       </c>
     </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
     <row r="4" spans="1:5">
       <c r="E4" s="2"/>
     </row>
@@ -3116,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3131,7 +3169,7 @@
     <col min="23" max="23" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3199,10 +3237,13 @@
         <v>422</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
+        <v>487</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3273,7 +3314,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -3341,7 +3382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3409,7 +3450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -3477,7 +3518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -3546,7 +3587,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3614,7 +3655,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3682,7 +3723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -3750,7 +3791,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -6792,7 +6833,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -6893,7 +6934,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -6995,7 +7036,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -7048,7 +7089,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -7106,7 +7147,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>
@@ -8892,7 +8933,7 @@
         <v>21</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>73</v>
@@ -8911,15 +8952,15 @@
         <v>60</v>
       </c>
       <c r="I95" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y95" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y95" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z95" s="7"/>
       <c r="AA95" s="12"/>
       <c r="AB95" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="96" spans="1:28" ht="18.95" customHeight="1">
@@ -8930,7 +8971,7 @@
         <v>248</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>73</v>
@@ -8949,15 +8990,15 @@
         <v>60</v>
       </c>
       <c r="I96" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y96" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y96" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z96" s="7"/>
       <c r="AA96" s="12"/>
       <c r="AB96" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="18.95" customHeight="1">
@@ -8968,7 +9009,7 @@
         <v>262</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>73</v>
@@ -8987,15 +9028,15 @@
         <v>60</v>
       </c>
       <c r="I97" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y97" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y97" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z97" s="7"/>
       <c r="AA97" s="12"/>
       <c r="AB97" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="18.95" customHeight="1">
@@ -9006,7 +9047,7 @@
         <v>143</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>73</v>
@@ -9025,15 +9066,15 @@
         <v>60</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y98" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y98" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z98" s="7"/>
       <c r="AA98" s="12"/>
       <c r="AB98" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="18.95" customHeight="1">
@@ -9044,7 +9085,7 @@
         <v>187</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>73</v>
@@ -9063,15 +9104,15 @@
         <v>60</v>
       </c>
       <c r="I99" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y99" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y99" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z99" s="7"/>
       <c r="AA99" s="12"/>
       <c r="AB99" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="18.95" customHeight="1">
@@ -9082,7 +9123,7 @@
         <v>186</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>73</v>
@@ -9101,15 +9142,15 @@
         <v>60</v>
       </c>
       <c r="I100" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y100" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y100" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z100" s="7"/>
       <c r="AA100" s="12"/>
       <c r="AB100" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="18.95" customHeight="1">
@@ -9120,7 +9161,7 @@
         <v>23</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>73</v>
@@ -9139,15 +9180,15 @@
         <v>60</v>
       </c>
       <c r="I101" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y101" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y101" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z101" s="7"/>
       <c r="AA101" s="12"/>
       <c r="AB101" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="18.95" customHeight="1">
@@ -9158,7 +9199,7 @@
         <v>188</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>73</v>
@@ -9177,15 +9218,15 @@
         <v>60</v>
       </c>
       <c r="I102" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y102" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y102" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z102" s="7"/>
       <c r="AA102" s="12"/>
       <c r="AB102" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="18.95" customHeight="1">
@@ -9196,7 +9237,7 @@
         <v>167</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>73</v>
@@ -9215,15 +9256,15 @@
         <v>60</v>
       </c>
       <c r="I103" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y103" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y103" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z103" s="7"/>
       <c r="AA103" s="12"/>
       <c r="AB103" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="18.95" customHeight="1">
@@ -9234,7 +9275,7 @@
         <v>266</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>73</v>
@@ -9253,15 +9294,15 @@
         <v>60</v>
       </c>
       <c r="I104" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y104" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y104" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z104" s="7"/>
       <c r="AA104" s="12"/>
       <c r="AB104" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="18.95" customHeight="1">
@@ -9272,7 +9313,7 @@
         <v>191</v>
       </c>
       <c r="C105" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>73</v>
@@ -9291,15 +9332,15 @@
         <v>60</v>
       </c>
       <c r="I105" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y105" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y105" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z105" s="7"/>
       <c r="AA105" s="12"/>
       <c r="AB105" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="18.95" customHeight="1">
@@ -9310,7 +9351,7 @@
         <v>267</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>73</v>
@@ -9329,15 +9370,15 @@
         <v>60</v>
       </c>
       <c r="I106" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y106" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y106" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z106" s="7"/>
       <c r="AA106" s="12"/>
       <c r="AB106" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="18.95" customHeight="1">
@@ -9348,7 +9389,7 @@
         <v>389</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>73</v>
@@ -9367,15 +9408,15 @@
         <v>60</v>
       </c>
       <c r="I107" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y107" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y107" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z107" s="7"/>
       <c r="AA107" s="12"/>
       <c r="AB107" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="18.95" customHeight="1">
@@ -9386,7 +9427,7 @@
         <v>189</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>73</v>
@@ -9405,15 +9446,15 @@
         <v>60</v>
       </c>
       <c r="I108" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y108" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y108" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z108" s="7"/>
       <c r="AA108" s="12"/>
       <c r="AB108" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="18.95" customHeight="1">
@@ -9424,7 +9465,7 @@
         <v>281</v>
       </c>
       <c r="C109" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>73</v>
@@ -9443,15 +9484,15 @@
         <v>60</v>
       </c>
       <c r="I109" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y109" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y109" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z109" s="7"/>
       <c r="AA109" s="12"/>
       <c r="AB109" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="18.95" customHeight="1">
@@ -9462,7 +9503,7 @@
         <v>22</v>
       </c>
       <c r="C110" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>73</v>
@@ -9481,15 +9522,15 @@
         <v>60</v>
       </c>
       <c r="I110" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y110" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y110" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z110" s="7"/>
       <c r="AA110" s="12"/>
       <c r="AB110" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="18.95" customHeight="1">
@@ -9500,7 +9541,7 @@
         <v>288</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>73</v>
@@ -9519,15 +9560,15 @@
         <v>60</v>
       </c>
       <c r="I111" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y111" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y111" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z111" s="7"/>
       <c r="AA111" s="12"/>
       <c r="AB111" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="18.95" customHeight="1">
@@ -9538,7 +9579,7 @@
         <v>291</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>73</v>
@@ -9557,15 +9598,15 @@
         <v>60</v>
       </c>
       <c r="I112" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y112" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y112" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z112" s="7"/>
       <c r="AA112" s="12"/>
       <c r="AB112" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="18.95" customHeight="1">
@@ -9576,7 +9617,7 @@
         <v>190</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>73</v>
@@ -9595,15 +9636,15 @@
         <v>60</v>
       </c>
       <c r="I113" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y113" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="Y113" s="5" t="s">
-        <v>513</v>
       </c>
       <c r="Z113" s="7"/>
       <c r="AA113" s="12"/>
       <c r="AB113" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -10168,13 +10209,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H20" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B20&amp;"s and associated provenance for a patient")</f>
@@ -10201,13 +10242,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H21" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B21&amp;" and its associated provenance")</f>
@@ -10591,13 +10632,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H35" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B35&amp;"s and associated provenance for a patient")</f>
@@ -10624,13 +10665,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H36" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B36&amp;" and its associated provenance")</f>
@@ -10780,13 +10821,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H41" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B41&amp;"s and associated provenance for a patient")</f>
@@ -10813,13 +10854,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H42" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B42&amp;" and its associated provenance")</f>
@@ -10861,7 +10902,7 @@
         <v>351</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -10876,22 +10917,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D44" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="H44" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="I44" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="J44" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -10906,22 +10947,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D45" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="H45" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="I45" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -10998,13 +11039,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H48" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B48&amp;"s and associated provenance for a patient")</f>
@@ -11031,13 +11072,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H49" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B49&amp;" and its associated provenance")</f>
@@ -11219,13 +11260,13 @@
         <v>197</v>
       </c>
       <c r="D55" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H55" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B55&amp;"s and associated provenance for a patient")</f>
@@ -11251,13 +11292,13 @@
         <v>197</v>
       </c>
       <c r="D56" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H56" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B56&amp;" and its associated provenance")</f>
@@ -11433,13 +11474,13 @@
         <v>198</v>
       </c>
       <c r="D62" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H62" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B62&amp;"s and associated provenance for a patient")</f>
@@ -11465,13 +11506,13 @@
         <v>198</v>
       </c>
       <c r="D63" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H63" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B63&amp;" and its associated provenance")</f>
@@ -11560,13 +11601,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D66" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H66" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B66&amp;"s and associated provenance for a patient")</f>
@@ -11593,13 +11634,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D67" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H67" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B67&amp;" and its associated provenance")</f>
@@ -11626,7 +11667,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>73</v>
@@ -11635,16 +11676,16 @@
         <v>111</v>
       </c>
       <c r="G68" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="H68" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -11659,7 +11700,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>73</v>
@@ -11668,7 +11709,7 @@
         <v>111</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>194</v>
@@ -11677,7 +11718,7 @@
         <v>460</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -11692,7 +11733,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>73</v>
@@ -11701,7 +11742,7 @@
         <v>111</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>194</v>
@@ -11710,7 +11751,7 @@
         <v>460</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -11725,7 +11766,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>73</v>
@@ -11734,7 +11775,7 @@
         <v>229</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>244</v>
@@ -11743,7 +11784,7 @@
         <v>461</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -11758,13 +11799,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D72" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H72" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B72&amp;"s and associated provenance for a patient")</f>
@@ -11791,13 +11832,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D73" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H73" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B73&amp;" and its associated provenance")</f>
@@ -11817,7 +11858,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C74" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11848,7 +11889,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C75" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11978,13 +12019,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D79" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H79" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B79&amp;"s and associated provenance for a patient")</f>
@@ -12011,13 +12052,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D80" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H80" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B80&amp;" and its associated provenance")</f>
@@ -12052,13 +12093,13 @@
         <v>111</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J81" s="5" t="s">
         <v>347</v>
@@ -12084,13 +12125,13 @@
         <v>111</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12147,13 +12188,13 @@
         <v>229</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J84" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12231,13 +12272,13 @@
         <v>451</v>
       </c>
       <c r="D87" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H87" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B87&amp;"s and associated provenance for a patient")</f>
@@ -12263,13 +12304,13 @@
         <v>451</v>
       </c>
       <c r="D88" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H88" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B88&amp;" and its associated provenance")</f>
@@ -12425,13 +12466,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="D93" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H93" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B93&amp;"s and associated provenance for a patient")</f>
@@ -12458,13 +12499,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="D94" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H94" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B94&amp;" and its associated provenance")</f>
@@ -12524,13 +12565,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D96" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H96" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B96&amp;"s and associated provenance for a patient")</f>
@@ -12557,13 +12598,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D97" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H97" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B97&amp;" and its associated provenance")</f>
@@ -12622,13 +12663,13 @@
         <v>297</v>
       </c>
       <c r="D99" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H99" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B99&amp;"s and associated provenance for a patient")</f>
@@ -12654,13 +12695,13 @@
         <v>297</v>
       </c>
       <c r="D100" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H100" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B100&amp;" and its associated provenance")</f>
@@ -12695,13 +12736,13 @@
         <v>111</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J101" s="5" t="str">
         <f t="shared" ref="J101" si="9">"Fetches a bundle of all "&amp;B101&amp;" resources for the specified "&amp;SUBSTITUTE(D101,","," and ")</f>
@@ -12728,13 +12769,13 @@
         <v>111</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>300</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J102" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -12761,7 +12802,7 @@
         <v>111</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>303</v>
@@ -12794,13 +12835,13 @@
         <v>229</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H104" s="5" t="s">
         <v>306</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J104" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -12848,13 +12889,13 @@
         <v>345</v>
       </c>
       <c r="D106" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H106" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B106&amp;"s and associated provenance for a patient")</f>
@@ -12880,13 +12921,13 @@
         <v>345</v>
       </c>
       <c r="D107" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H107" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B107&amp;" and its associated provenance")</f>
@@ -13100,13 +13141,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D114" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H114" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B114&amp;"s and associated provenance for a patient")</f>
@@ -13133,13 +13174,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D115" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H115" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B115&amp;" and its associated provenance")</f>
@@ -13194,13 +13235,13 @@
         <v>475</v>
       </c>
       <c r="D117" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H117" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B117&amp;"s and associated provenance for a patient")</f>
@@ -13226,13 +13267,13 @@
         <v>475</v>
       </c>
       <c r="D118" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H118" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B118&amp;" and its associated provenance")</f>
@@ -13258,13 +13299,13 @@
         <v>475</v>
       </c>
       <c r="D119" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H119" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B119&amp;"s and associated provenance for a patient")</f>
@@ -13290,13 +13331,13 @@
         <v>475</v>
       </c>
       <c r="D120" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H120" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B120&amp;" and its associated provenance")</f>
@@ -13322,13 +13363,13 @@
         <v>475</v>
       </c>
       <c r="D121" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F121" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H121" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B121&amp;"s and associated provenance for a patient")</f>
@@ -13354,13 +13395,13 @@
         <v>475</v>
       </c>
       <c r="D122" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H122" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B122&amp;" and its associated provenance")</f>
@@ -13386,13 +13427,13 @@
         <v>475</v>
       </c>
       <c r="D123" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F123" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H123" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B123&amp;"s and associated provenance for a patient")</f>
@@ -13418,13 +13459,13 @@
         <v>475</v>
       </c>
       <c r="D124" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H124" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B124&amp;" and its associated provenance")</f>
@@ -13450,13 +13491,13 @@
         <v>475</v>
       </c>
       <c r="D125" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F125" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="H125" s="5" t="str">
         <f>"support searching for all "&amp;LOWER(B125&amp;"s and associated provenance for a patient")</f>
@@ -13482,13 +13523,13 @@
         <v>475</v>
       </c>
       <c r="D126" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="H126" s="5" t="str">
         <f>"support searching for a "&amp;LOWER(B126&amp;" and its associated provenance")</f>

</xml_diff>

<commit_message>
preapply GF24089, GF#24090, GF#24106#
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD7708D-6390-4AFB-8844-64DAED169763}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E605F9-DE9C-4594-B712-7BA0C169375A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21585" yWindow="2040" windowWidth="18900" windowHeight="11055" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19755" yWindow="4170" windowWidth="18900" windowHeight="11055" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="520">
   <si>
     <t>Element</t>
   </si>
@@ -1705,6 +1705,12 @@
   </si>
   <si>
     <t>Provenance:target</t>
+  </si>
+  <si>
+    <t>doc_Observation</t>
+  </si>
+  <si>
+    <t>The conformance expectations for Composite Searches differ by profile.  See the Quick Start section for profile specific expectations.</t>
   </si>
 </sst>
 </file>
@@ -2254,7 +2260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -3166,10 +3172,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3177,11 +3183,13 @@
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
     <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="8.85546875" style="1"/>
+    <col min="24" max="24" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3234,28 +3242,31 @@
         <v>417</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>422</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3307,9 +3318,6 @@
       <c r="Q2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
       <c r="S2" t="s">
         <v>32</v>
       </c>
@@ -3322,11 +3330,14 @@
       <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="X2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="285">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -3345,6 +3356,9 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>519</v>
+      </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
@@ -3375,8 +3389,8 @@
       <c r="Q3" t="s">
         <v>12</v>
       </c>
-      <c r="R3" t="s">
-        <v>12</v>
+      <c r="R3" s="2" t="s">
+        <v>519</v>
       </c>
       <c r="S3" t="s">
         <v>12</v>
@@ -3390,11 +3404,14 @@
       <c r="V3" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="X3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3443,9 +3460,6 @@
       <c r="Q4" t="s">
         <v>12</v>
       </c>
-      <c r="R4" t="s">
-        <v>12</v>
-      </c>
       <c r="S4" t="s">
         <v>12</v>
       </c>
@@ -3458,11 +3472,14 @@
       <c r="V4" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="X4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -3511,9 +3528,6 @@
       <c r="Q5" t="s">
         <v>73</v>
       </c>
-      <c r="R5" t="s">
-        <v>73</v>
-      </c>
       <c r="S5" t="s">
         <v>73</v>
       </c>
@@ -3526,11 +3540,14 @@
       <c r="V5" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="W5" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -3580,9 +3597,6 @@
       <c r="Q6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="S6" s="1" t="s">
         <v>32</v>
       </c>
@@ -3592,14 +3606,17 @@
       <c r="U6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="X6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3648,9 +3665,6 @@
       <c r="Q7" t="s">
         <v>32</v>
       </c>
-      <c r="R7" t="s">
-        <v>32</v>
-      </c>
       <c r="S7" t="s">
         <v>32</v>
       </c>
@@ -3663,11 +3677,14 @@
       <c r="V7" t="s">
         <v>32</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="X7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3716,9 +3733,6 @@
       <c r="Q8" t="s">
         <v>32</v>
       </c>
-      <c r="R8" t="s">
-        <v>32</v>
-      </c>
       <c r="S8" t="s">
         <v>32</v>
       </c>
@@ -3731,11 +3745,14 @@
       <c r="V8" t="s">
         <v>32</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="X8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -3784,9 +3801,6 @@
       <c r="Q9" t="s">
         <v>73</v>
       </c>
-      <c r="R9" t="s">
-        <v>73</v>
-      </c>
       <c r="S9" t="s">
         <v>73</v>
       </c>
@@ -3799,11 +3813,14 @@
       <c r="V9" t="s">
         <v>73</v>
       </c>
-      <c r="W9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="W9" t="s">
+        <v>73</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3852,9 +3869,6 @@
       <c r="Q10" t="s">
         <v>32</v>
       </c>
-      <c r="R10" t="s">
-        <v>32</v>
-      </c>
       <c r="S10" t="s">
         <v>32</v>
       </c>
@@ -3867,7 +3881,10 @@
       <c r="V10" t="s">
         <v>32</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" t="s">
+        <v>32</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3943,10 +3960,10 @@
   <dimension ref="A1:AB94"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95:XFD113"/>
+      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -6422,7 +6439,7 @@
         <v>73</v>
       </c>
       <c r="E48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -9014,7 +9031,7 @@
         <v>163</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <f t="shared" ref="C2:C39" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -9027,7 +9044,7 @@
         <v>105</v>
       </c>
       <c r="J2" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
+        <f t="shared" ref="J2:J32" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
@@ -9039,7 +9056,7 @@
         <v>163</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -9052,7 +9069,7 @@
         <v>107</v>
       </c>
       <c r="J3" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B3&amp;" resources matching the specified "&amp;SUBSTITUTE(D3,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
@@ -9064,7 +9081,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B4)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -9077,7 +9094,7 @@
         <v>107</v>
       </c>
       <c r="J4" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B4&amp;" resources matching the specified "&amp;SUBSTITUTE(D4,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
@@ -9089,7 +9106,7 @@
         <v>163</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B5)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -9102,7 +9119,7 @@
         <v>105</v>
       </c>
       <c r="J5" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B5&amp;" resources matching the specified "&amp;SUBSTITUTE(D5,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
@@ -9114,7 +9131,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -9133,7 +9150,7 @@
         <v>331</v>
       </c>
       <c r="J6" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B6&amp;" resources matching the specified "&amp;SUBSTITUTE(D6,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
@@ -9145,7 +9162,7 @@
         <v>163</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -9158,7 +9175,7 @@
         <v>111</v>
       </c>
       <c r="J7" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B7&amp;" resources matching the specified "&amp;SUBSTITUTE(D7,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
@@ -9170,7 +9187,7 @@
         <v>163</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B8)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -9183,7 +9200,7 @@
         <v>111</v>
       </c>
       <c r="J8" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B8&amp;" resources matching the specified "&amp;SUBSTITUTE(D8,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
@@ -9195,7 +9212,7 @@
         <v>163</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B9)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -9209,7 +9226,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B9&amp;" resources matching the specified "&amp;SUBSTITUTE(D9,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
@@ -9221,7 +9238,7 @@
         <v>163</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B10)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -9236,7 +9253,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B10&amp;" resources matching the specified "&amp;SUBSTITUTE(D10,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
@@ -9248,7 +9265,7 @@
         <v>163</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B11)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -9262,7 +9279,7 @@
       </c>
       <c r="H11" s="5"/>
       <c r="J11" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B11&amp;" resources matching the specified "&amp;SUBSTITUTE(D11,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
@@ -9274,7 +9291,7 @@
         <v>163</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B12)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -9287,7 +9304,7 @@
         <v>58</v>
       </c>
       <c r="J12" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B12&amp;" resources matching the specified "&amp;SUBSTITUTE(D12,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
@@ -9299,7 +9316,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B13)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -9318,7 +9335,7 @@
         <v>332</v>
       </c>
       <c r="J13" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B13&amp;" resources matching the specified "&amp;SUBSTITUTE(D13,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
@@ -9330,7 +9347,7 @@
         <v>163</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B14)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -9343,7 +9360,7 @@
         <v>107</v>
       </c>
       <c r="J14" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B14&amp;" resources matching the specified "&amp;SUBSTITUTE(D14,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
@@ -9355,7 +9372,7 @@
         <v>163</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B15)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -9368,7 +9385,7 @@
         <v>105</v>
       </c>
       <c r="J15" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B15&amp;" resources matching the specified "&amp;SUBSTITUTE(D15,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
@@ -9380,7 +9397,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B16)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -9399,7 +9416,7 @@
         <v>333</v>
       </c>
       <c r="J16" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B16&amp;" resources matching the specified "&amp;SUBSTITUTE(D16,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
@@ -9411,7 +9428,7 @@
         <v>163</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B17)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -9425,7 +9442,7 @@
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B17&amp;" resources matching the specified "&amp;SUBSTITUTE(D17,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
@@ -9437,7 +9454,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B18)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -9456,7 +9473,7 @@
         <v>334</v>
       </c>
       <c r="J18" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B18&amp;" resources matching the specified "&amp;SUBSTITUTE(D18,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
@@ -9468,7 +9485,7 @@
         <v>163</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -9483,7 +9500,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B19&amp;" resources matching the specified "&amp;SUBSTITUTE(D19,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
@@ -9495,7 +9512,7 @@
         <v>164</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B20)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -9509,7 +9526,7 @@
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B20&amp;" resources matching the specified "&amp;SUBSTITUTE(D20,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
@@ -9521,7 +9538,7 @@
         <v>164</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -9534,7 +9551,7 @@
         <v>128</v>
       </c>
       <c r="J21" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B21&amp;" resources matching the specified "&amp;SUBSTITUTE(D21,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
@@ -9546,7 +9563,7 @@
         <v>164</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B22)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -9560,7 +9577,7 @@
       </c>
       <c r="H22" s="5"/>
       <c r="J22" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B22&amp;" resources matching the specified "&amp;SUBSTITUTE(D22,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
@@ -9572,7 +9589,7 @@
         <v>164</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B23)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -9587,7 +9604,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B23&amp;" resources matching the specified "&amp;SUBSTITUTE(D23,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
@@ -9599,7 +9616,7 @@
         <v>164</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B24)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -9614,7 +9631,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B24&amp;" resources matching the specified "&amp;SUBSTITUTE(D24,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
@@ -9626,7 +9643,7 @@
         <v>164</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -9641,7 +9658,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B25&amp;" resources matching the specified "&amp;SUBSTITUTE(D25,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
@@ -9653,7 +9670,7 @@
         <v>164</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -9666,7 +9683,7 @@
         <v>132</v>
       </c>
       <c r="J26" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B26&amp;" resources matching the specified "&amp;SUBSTITUTE(D26,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
@@ -9678,7 +9695,7 @@
         <v>164</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B27)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -9691,7 +9708,7 @@
         <v>58</v>
       </c>
       <c r="J27" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the specified "&amp;SUBSTITUTE(D27,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
@@ -9703,7 +9720,7 @@
         <v>164</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B28)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -9716,7 +9733,7 @@
         <v>132</v>
       </c>
       <c r="J28" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B28&amp;" resources matching the specified "&amp;SUBSTITUTE(D28,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
@@ -9728,7 +9745,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B29)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -9747,7 +9764,7 @@
         <v>185</v>
       </c>
       <c r="J29" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B29&amp;" resources matching the specified "&amp;SUBSTITUTE(D29,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
@@ -9759,7 +9776,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B30)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -9778,7 +9795,7 @@
         <v>182</v>
       </c>
       <c r="J30" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B30&amp;" resources matching the specified "&amp;SUBSTITUTE(D30,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
@@ -9790,7 +9807,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -9809,7 +9826,7 @@
         <v>184</v>
       </c>
       <c r="J31" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the specified "&amp;SUBSTITUTE(D31,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
@@ -9821,7 +9838,7 @@
         <v>22</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B32)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -9840,7 +9857,7 @@
         <v>183</v>
       </c>
       <c r="J32" s="5" t="str">
-        <f>"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
+        <f t="shared" si="1"/>
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
@@ -9852,7 +9869,7 @@
         <v>143</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B33)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -9885,7 +9902,7 @@
         <v>143</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -9915,7 +9932,7 @@
         <v>143</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -9945,7 +9962,7 @@
         <v>143</v>
       </c>
       <c r="C36" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B36)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -9975,7 +9992,7 @@
         <v>21</v>
       </c>
       <c r="C37" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B37)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -10005,7 +10022,7 @@
         <v>167</v>
       </c>
       <c r="C38" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -10036,7 +10053,7 @@
         <v>167</v>
       </c>
       <c r="C39" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B39)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -10373,7 +10390,7 @@
         <v>188</v>
       </c>
       <c r="C50" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
+        <f t="shared" ref="C50:C60" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -10404,7 +10421,7 @@
         <v>188</v>
       </c>
       <c r="C51" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B51)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -10435,7 +10452,7 @@
         <v>189</v>
       </c>
       <c r="C52" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B52)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -10468,7 +10485,7 @@
         <v>189</v>
       </c>
       <c r="C53" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B53)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -10501,7 +10518,7 @@
         <v>189</v>
       </c>
       <c r="C54" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -10534,7 +10551,7 @@
         <v>189</v>
       </c>
       <c r="C55" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B55)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -10567,7 +10584,7 @@
         <v>499</v>
       </c>
       <c r="C56" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -10598,7 +10615,7 @@
         <v>499</v>
       </c>
       <c r="C57" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B57)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -10628,7 +10645,7 @@
         <v>190</v>
       </c>
       <c r="C58" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B58)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -10659,7 +10676,7 @@
         <v>190</v>
       </c>
       <c r="C59" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B59)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -10690,7 +10707,7 @@
         <v>190</v>
       </c>
       <c r="C60" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B60)</f>
+        <f t="shared" si="2"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -11266,7 +11283,7 @@
         <v>186</v>
       </c>
       <c r="C78" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
+        <f t="shared" ref="C78:C83" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -11297,7 +11314,7 @@
         <v>313</v>
       </c>
       <c r="C79" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -11326,7 +11343,7 @@
         <v>186</v>
       </c>
       <c r="C80" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B80)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -11359,7 +11376,7 @@
         <v>186</v>
       </c>
       <c r="C81" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B81)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -11392,7 +11409,7 @@
         <v>186</v>
       </c>
       <c r="C82" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -11422,7 +11439,7 @@
         <v>186</v>
       </c>
       <c r="C83" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
+        <f t="shared" si="3"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" s="1" t="s">

</xml_diff>

<commit_message>
healthedata1 Preapply GF#24108 and GF#24446
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/source/source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D6905-E659-AE4C-8EA4-953AC3CC76FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BD0050-5AE4-5F4E-9E1A-7ACFAA671234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1707,7 +1707,7 @@
     <t>doc_Observation</t>
   </si>
   <si>
-    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item~GET [base]/Condition?patient=1032702&amp;category=http://hl7.org/fhir/us/core/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
   </si>
 </sst>
 </file>
@@ -8962,8 +8962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="H30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
healthedata1 Apply trackers: GF#24632 fix typo when pre applying GF#23854 in revinclude for capstatements should be SHALL and added to Allergy
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2C364-C81E-4822-9BAD-CD022B223787}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF026AA-36C7-41E4-ACFA-16C86B73A207}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="520">
   <si>
     <t>Element</t>
   </si>
@@ -1521,9 +1521,6 @@
   </si>
   <si>
     <t>GET [base]/Goal?patient=1137192&amp;target-date=ge2015-01-14&amp;target-date=le2019-01-14</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;status=active&amp;_include=MedicationRequest:medication</t>
   </si>
   <si>
     <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active~GET [base]/MedicationStatement?patient=1137192&amp;status=active&amp;_include=MedicationStatement:medication</t>
@@ -1614,15 +1611,9 @@
     <t>patient,intent</t>
   </si>
   <si>
-    <t>intent=http://hl7.org/fhir/CodeSystem/medicationrequest-intent|order</t>
-  </si>
-  <si>
     <t>support searching for all medications that have been prescribed to a patient. See the [Medication List Guidance] section for guidance on accessing a patient medications. The server application represents the medication using either an inline code or a contained or external reference to the Medication resource.</t>
   </si>
   <si>
-    <t>GET [base]/MedicationRequest?patient=14676&amp;intent=http://hl7.org/fhir/CodeSystem/medicationrequest-intent|order~GET [base]/MedicationRequest?patient=14676&amp;intent=http://hl7.org/fhir/CodeSystem/medicationrequest-intent|order&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
     <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent code = `order`</t>
   </si>
   <si>
@@ -1707,7 +1698,19 @@
     <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item~GET [base]/Condition?patient=1032702&amp;category=http://hl7.org/fhir/us/core/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
   </si>
   <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
+    <t>intent=order</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=14676&amp;intent=order~GET [base]/MedicationRequest?patient=14676&amp;intent=order&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;encounter=Encounter/123~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;&amp;encounter=Encounter/123&amp;_include=MedicationRequest:medication</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2224,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2338,10 +2341,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -2488,10 +2491,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -2623,10 +2626,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>467</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2638,10 +2641,10 @@
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>481</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -2680,16 +2683,16 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -2703,11 +2706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="U8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V13" sqref="V13"/>
+      <selection pane="bottomRight" activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
@@ -2810,8 +2813,9 @@
       <c r="D2"/>
       <c r="F2"/>
       <c r="R2"/>
+      <c r="V2" s="17"/>
       <c r="W2" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="X2" t="s">
         <v>20</v>
@@ -2824,8 +2828,9 @@
       <c r="B3" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V3" s="17"/>
       <c r="W3" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="17.25" customHeight="1">
@@ -2835,8 +2840,9 @@
       <c r="B4" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V4" s="17"/>
       <c r="W4" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="17.25" customHeight="1">
@@ -2846,8 +2852,9 @@
       <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V5" s="17"/>
       <c r="W5" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="X5" t="s">
         <v>24</v>
@@ -2860,8 +2867,9 @@
       <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V6" s="17"/>
       <c r="W6" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
@@ -2871,8 +2879,9 @@
       <c r="B7" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V7" s="17"/>
       <c r="W7" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
@@ -2885,8 +2894,9 @@
       <c r="C8" s="2" t="s">
         <v>448</v>
       </c>
+      <c r="V8" s="17"/>
       <c r="W8" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
@@ -2896,8 +2906,9 @@
       <c r="B9" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V9" s="17"/>
       <c r="W9" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
@@ -2907,8 +2918,9 @@
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V10" s="17"/>
       <c r="W10" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
@@ -2918,8 +2930,9 @@
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V11" s="17"/>
       <c r="W11" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1">
@@ -2929,8 +2942,9 @@
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V12" s="17"/>
       <c r="W12" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1">
@@ -2943,8 +2957,9 @@
       <c r="C13" s="2" t="s">
         <v>435</v>
       </c>
+      <c r="V13" s="17"/>
       <c r="W13" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="17.25" customHeight="1">
@@ -2955,30 +2970,32 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="U14" s="7" t="s">
         <v>219</v>
       </c>
+      <c r="V14" s="17"/>
       <c r="W14" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>432</v>
       </c>
+      <c r="V15" s="17"/>
       <c r="W15" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17.25" customHeight="1">
@@ -2988,8 +3005,9 @@
       <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V16" s="17"/>
       <c r="W16" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="17.25" customHeight="1">
@@ -2999,8 +3017,9 @@
       <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V17" s="17"/>
       <c r="W17" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="17.25" customHeight="1">
@@ -3010,8 +3029,9 @@
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V18" s="17"/>
       <c r="W18" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="17.25" customHeight="1">
@@ -3021,8 +3041,9 @@
       <c r="B19" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V19" s="17"/>
       <c r="W19" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="17.25" customHeight="1">
@@ -3035,8 +3056,9 @@
       <c r="U20" s="1" t="s">
         <v>295</v>
       </c>
+      <c r="V20" s="17"/>
       <c r="W20" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="17.25" customHeight="1">
@@ -3046,13 +3068,14 @@
       <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="V21" s="17"/>
       <c r="W21" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="15">
       <c r="A22" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
@@ -3061,7 +3084,7 @@
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
@@ -3139,24 +3162,24 @@
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3171,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3206,7 +3229,7 @@
         <v>406</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>407</v>
@@ -3239,7 +3262,7 @@
         <v>416</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>417</v>
@@ -3257,10 +3280,10 @@
         <v>421</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3283,7 +3306,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -3904,12 +3927,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -3918,7 +3941,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -3927,7 +3950,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -3936,7 +3959,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -3953,7 +3976,7 @@
   <dimension ref="A1:AB94"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
@@ -6855,7 +6878,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -6956,7 +6979,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -7058,7 +7081,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -7111,7 +7134,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -7169,7 +7192,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>
@@ -8962,8 +8985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -9908,7 +9931,7 @@
         <v>155</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>151</v>
@@ -10001,7 +10024,7 @@
         <v>351</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -10446,7 +10469,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>73</v>
@@ -10455,16 +10478,16 @@
         <v>111</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>487</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -10479,7 +10502,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>73</v>
@@ -10488,16 +10511,16 @@
         <v>111</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>487</v>
+        <v>515</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>459</v>
+        <v>517</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -10512,7 +10535,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>73</v>
@@ -10521,16 +10544,16 @@
         <v>111</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>487</v>
+        <v>515</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>459</v>
+        <v>519</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -10545,7 +10568,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>73</v>
@@ -10554,7 +10577,7 @@
         <v>229</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>487</v>
+        <v>515</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>244</v>
@@ -10563,7 +10586,7 @@
         <v>518</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -10571,7 +10594,7 @@
         <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -10590,7 +10613,7 @@
         <v>196</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J56" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -10602,7 +10625,7 @@
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
@@ -10621,7 +10644,7 @@
         <v>245</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>247</v>
@@ -10740,13 +10763,13 @@
         <v>111</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>347</v>
@@ -10772,13 +10795,13 @@
         <v>111</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -10835,13 +10858,13 @@
         <v>229</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="J64" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -10967,7 +10990,7 @@
         <v>255</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>259</v>
@@ -11031,7 +11054,7 @@
         <v>254</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>261</v>
@@ -11123,13 +11146,13 @@
         <v>111</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")</f>
@@ -11156,13 +11179,13 @@
         <v>111</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>300</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11189,7 +11212,7 @@
         <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>303</v>
@@ -11222,13 +11245,13 @@
         <v>229</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>306</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11460,7 +11483,7 @@
         <v>266</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
FHIR-25035 update search parameters and quick start
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/source/source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB20138-C988-4297-982E-1EB7220B78AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255C1E46-1B10-614C-9D2F-5EC5D3882EE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="375" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-61360" yWindow="-1500" windowWidth="28800" windowHeight="17540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sp_combos!$B$1:$B$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sps!$A$1:$AB$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sps!$A$1:$AB$94</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="523">
   <si>
     <t>Element</t>
   </si>
@@ -1614,27 +1614,15 @@
     <t>support searching for all medications that have been prescribed to a patient. See the [Medication List Guidance] section for guidance on accessing a patient medications. The server application represents the medication using either an inline code or a contained or external reference to the Medication resource.</t>
   </si>
   <si>
-    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent code = `order`</t>
-  </si>
-  <si>
     <t>patient,intent,status</t>
   </si>
   <si>
-    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order` and status</t>
-  </si>
-  <si>
     <t>patient,intent,encounter</t>
   </si>
   <si>
-    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order` and encounter</t>
-  </si>
-  <si>
     <t>patient,intent,authoredon</t>
   </si>
   <si>
-    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order` and authoredon date</t>
-  </si>
-  <si>
     <t>!MedicationStatement</t>
   </si>
   <si>
@@ -1698,21 +1686,6 @@
     <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item~GET [base]/Condition?patient=1032702&amp;category=http://hl7.org/fhir/us/core/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
   </si>
   <si>
-    <t>intent=order</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=14676&amp;intent=order~GET [base]/MedicationRequest?patient=14676&amp;intent=order&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
-    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;encounter=Encounter/123~GET [base]/MedicationRequest?patient=1137192&amp;intent=order&amp;status=active&amp;&amp;encounter=Encounter/123&amp;_include=MedicationRequest:medication</t>
-  </si>
-  <si>
     <t>fhirVersion</t>
   </si>
   <si>
@@ -1720,13 +1693,40 @@
   </si>
   <si>
     <t>3.0.1</t>
+  </si>
+  <si>
+    <t>intent=order,plan</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=14676&amp;intent=order,plan~GET [base]/MedicationRequest?patient=14676&amp;intent=order,plan&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent code = `order,plan`</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and status</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;encounter=Encounter/123~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;&amp;encounter=Encounter/123&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and encounter</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and authoredon date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2194,17 +2194,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2212,23 +2212,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" customHeight="1">
+    <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2244,15 +2244,15 @@
         <v>444</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="141" customHeight="1">
+    <row r="8" spans="1:2" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="103.5" customHeight="1">
+    <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2289,9 +2289,9 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2312,15 +2312,15 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>366</v>
       </c>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>368</v>
       </c>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>472</v>
       </c>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>370</v>
       </c>
@@ -2394,7 +2394,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>372</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>297</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>375</v>
       </c>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>377</v>
       </c>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>379</v>
       </c>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>381</v>
       </c>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>382</v>
       </c>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>463</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>384</v>
       </c>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>386</v>
       </c>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>450</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>198</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>390</v>
       </c>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>250</v>
       </c>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>393</v>
       </c>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>395</v>
       </c>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>465</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1">
+    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>479</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="1" customFormat="1">
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>197</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="1" customFormat="1">
+    <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="1" customFormat="1">
+    <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>481</v>
       </c>
@@ -2738,22 +2738,22 @@
       <selection pane="bottomRight" activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1">
+    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -2840,13 +2840,13 @@
       <c r="R2"/>
       <c r="V2" s="17"/>
       <c r="W2" s="17" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="X2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17.25" customHeight="1">
+    <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>248</v>
       </c>
@@ -2855,10 +2855,10 @@
       </c>
       <c r="V3" s="17"/>
       <c r="W3" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>262</v>
       </c>
@@ -2867,10 +2867,10 @@
       </c>
       <c r="V4" s="17"/>
       <c r="W4" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>143</v>
       </c>
@@ -2879,13 +2879,13 @@
       </c>
       <c r="V5" s="17"/>
       <c r="W5" s="17" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="X5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>266</v>
       </c>
@@ -2894,10 +2894,10 @@
       </c>
       <c r="V6" s="17"/>
       <c r="W6" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>187</v>
       </c>
@@ -2906,10 +2906,10 @@
       </c>
       <c r="V7" s="17"/>
       <c r="W7" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>186</v>
       </c>
@@ -2921,10 +2921,10 @@
       </c>
       <c r="V8" s="17"/>
       <c r="W8" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2933,10 +2933,10 @@
       </c>
       <c r="V9" s="17"/>
       <c r="W9" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>188</v>
       </c>
@@ -2945,10 +2945,10 @@
       </c>
       <c r="V10" s="17"/>
       <c r="W10" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>167</v>
       </c>
@@ -2957,10 +2957,10 @@
       </c>
       <c r="V11" s="17"/>
       <c r="W11" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>267</v>
       </c>
@@ -2969,10 +2969,10 @@
       </c>
       <c r="V12" s="17"/>
       <c r="W12" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>388</v>
       </c>
@@ -2984,10 +2984,10 @@
       </c>
       <c r="V13" s="17"/>
       <c r="W13" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>189</v>
       </c>
@@ -3002,12 +3002,12 @@
       </c>
       <c r="V14" s="17"/>
       <c r="W14" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
@@ -3020,10 +3020,10 @@
       </c>
       <c r="V15" s="17"/>
       <c r="W15" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
@@ -3032,10 +3032,10 @@
       </c>
       <c r="V16" s="17"/>
       <c r="W16" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>281</v>
       </c>
@@ -3044,10 +3044,10 @@
       </c>
       <c r="V17" s="17"/>
       <c r="W17" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -3056,10 +3056,10 @@
       </c>
       <c r="V18" s="17"/>
       <c r="W18" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>288</v>
       </c>
@@ -3068,10 +3068,10 @@
       </c>
       <c r="V19" s="17"/>
       <c r="W19" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>291</v>
       </c>
@@ -3083,10 +3083,10 @@
       </c>
       <c r="V20" s="17"/>
       <c r="W20" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="17.25" customHeight="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>190</v>
       </c>
@@ -3095,10 +3095,10 @@
       </c>
       <c r="V21" s="17"/>
       <c r="W21" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" s="1" customFormat="1" ht="15">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>483</v>
       </c>
@@ -3107,27 +3107,27 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:23" s="1" customFormat="1" ht="15">
+    <row r="23" spans="1:23" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:23" ht="17.25" customHeight="1">
+    <row r="24" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:23" ht="17.25" customHeight="1">
+    <row r="25" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="17.25" customHeight="1">
+    <row r="56" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="17.25" customHeight="1">
+    <row r="59" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
@@ -3148,15 +3148,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90.75" thickBot="1">
+    <row r="2" spans="1:5" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>401</v>
       </c>
@@ -3190,24 +3190,24 @@
         <v>467</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3223,18 +3223,18 @@
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="1"/>
-    <col min="24" max="24" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" style="1"/>
+    <col min="24" max="24" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>416</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>417</v>
@@ -3308,10 +3308,10 @@
         <v>484</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3942,9 +3942,9 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>474</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>475</v>
       </c>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>476</v>
       </c>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>477</v>
       </c>
@@ -4000,45 +4000,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G72" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="73.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="73.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.85546875" style="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>146</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="18.95" customHeight="1" thickTop="1">
+    <row r="2" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="18.95" customHeight="1">
+    <row r="3" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="18.95" customHeight="1">
+    <row r="4" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="18.95" customHeight="1">
+    <row r="5" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="18.95" customHeight="1">
+    <row r="6" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="18.95" customHeight="1">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.95" customHeight="1">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="18.95" customHeight="1">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="18.95" customHeight="1">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="18.95" customHeight="1">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="18.95" customHeight="1">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="18.95" customHeight="1">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="18.95" customHeight="1">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="18.95" customHeight="1">
+    <row r="15" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="18.95" customHeight="1">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="18.95" customHeight="1">
+    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="18.95" customHeight="1">
+    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="18.95" customHeight="1">
+    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="18.95" customHeight="1">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="18.95" customHeight="1">
+    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="18.95" customHeight="1">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="18.95" customHeight="1">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="18.95" customHeight="1">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="18.95" customHeight="1">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="18.95" customHeight="1">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="18.95" customHeight="1">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18.95" customHeight="1">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="18.95" customHeight="1">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="18.95" customHeight="1">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="18.95" customHeight="1">
+    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="18.95" customHeight="1">
+    <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="18.95" customHeight="1">
+    <row r="33" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="18.95" customHeight="1">
+    <row r="34" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="18.95" customHeight="1">
+    <row r="35" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="18.95" customHeight="1">
+    <row r="36" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="18.95" customHeight="1">
+    <row r="37" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="18.95" customHeight="1">
+    <row r="38" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="18.95" customHeight="1">
+    <row r="39" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="18.95" customHeight="1">
+    <row r="40" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="18.95" customHeight="1">
+    <row r="41" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="18.95" customHeight="1">
+    <row r="42" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="18.95" customHeight="1">
+    <row r="43" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="18.95" customHeight="1">
+    <row r="44" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="18.95" customHeight="1">
+    <row r="45" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="18.95" customHeight="1">
+    <row r="46" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="18.95" customHeight="1">
+    <row r="47" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="18.95" customHeight="1">
+    <row r="48" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="18.95" customHeight="1">
+    <row r="49" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="18.95" customHeight="1">
+    <row r="50" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="18.95" customHeight="1">
+    <row r="51" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="18.95" customHeight="1">
+    <row r="52" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="18.95" customHeight="1">
+    <row r="53" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="18.95" customHeight="1">
+    <row r="54" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="18.95" customHeight="1">
+    <row r="55" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="18.95" customHeight="1">
+    <row r="56" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -6930,6 +6930,9 @@
       </c>
       <c r="K56" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>57</v>
@@ -6945,7 +6948,7 @@
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="18.95" customHeight="1">
+    <row r="57" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>54</v>
       </c>
@@ -6996,7 +6999,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="18.95" customHeight="1">
+    <row r="58" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -7004,7 +7007,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -7047,7 +7050,7 @@
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="18.95" customHeight="1">
+    <row r="59" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -7101,12 +7104,12 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="18.95" customHeight="1">
+    <row r="60" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -7154,12 +7157,12 @@
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="18.95" customHeight="1">
+    <row r="61" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -7212,12 +7215,12 @@
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="18.95" customHeight="1">
+    <row r="62" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>
@@ -7266,7 +7269,7 @@
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="18.95" customHeight="1">
+    <row r="63" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -7319,7 +7322,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="18.95" customHeight="1">
+    <row r="64" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -7377,7 +7380,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="18.95" customHeight="1">
+    <row r="65" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -7431,7 +7434,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="18.95" customHeight="1">
+    <row r="66" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -7481,7 +7484,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="18.95" customHeight="1">
+    <row r="67" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -7534,7 +7537,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="18.95" customHeight="1">
+    <row r="68" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -7584,7 +7587,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="18.95" customHeight="1">
+    <row r="69" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -7634,7 +7637,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="18.95" customHeight="1">
+    <row r="70" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -7688,7 +7691,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="18.95" customHeight="1">
+    <row r="71" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -7747,7 +7750,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="18.95" customHeight="1">
+    <row r="72" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -7797,7 +7800,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="18.95" customHeight="1">
+    <row r="73" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -7844,7 +7847,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="18.95" customHeight="1">
+    <row r="74" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -7898,7 +7901,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="18.95" customHeight="1">
+    <row r="75" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -7957,7 +7960,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="18.95" customHeight="1">
+    <row r="76" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -8010,7 +8013,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="18.95" customHeight="1">
+    <row r="77" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -8069,7 +8072,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="18.95" customHeight="1">
+    <row r="78" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -8122,7 +8125,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="18.95" customHeight="1">
+    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -8181,7 +8184,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18.95" customHeight="1">
+    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -8227,7 +8230,7 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18.95" customHeight="1">
+    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -8281,7 +8284,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18.95" customHeight="1">
+    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18.95" customHeight="1">
+    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="18.95" customHeight="1">
+    <row r="84" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -8443,7 +8446,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="18.95" customHeight="1">
+    <row r="85" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -8497,7 +8500,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="18.95" customHeight="1">
+    <row r="86" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -8551,7 +8554,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="18.95" customHeight="1">
+    <row r="87" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -8605,7 +8608,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="18.95" customHeight="1">
+    <row r="88" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -8659,7 +8662,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="18.95" customHeight="1">
+    <row r="89" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -8713,7 +8716,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="18.95" customHeight="1">
+    <row r="90" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -8767,7 +8770,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="18.95" customHeight="1">
+    <row r="91" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -8824,7 +8827,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="18.95" customHeight="1">
+    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -8878,7 +8881,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="18.95" customHeight="1">
+    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -8935,7 +8938,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="18.95" customHeight="1">
+    <row r="94" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -8996,7 +8999,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <autoFilter ref="A1:AB94" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
@@ -9010,26 +9013,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="88.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="96.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="82.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -9061,7 +9064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -9086,7 +9089,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -9111,7 +9114,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -9136,7 +9139,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -9161,7 +9164,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -9192,7 +9195,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9217,7 +9220,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -9242,7 +9245,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -9268,7 +9271,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9295,7 +9298,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -9321,7 +9324,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -9346,7 +9349,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9377,7 +9380,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9402,7 +9405,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9427,7 +9430,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9458,7 +9461,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9484,7 +9487,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9515,7 +9518,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9542,7 +9545,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>21</v>
       </c>
@@ -9568,7 +9571,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>22</v>
       </c>
@@ -9593,7 +9596,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>23</v>
       </c>
@@ -9619,7 +9622,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -9646,7 +9649,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>25</v>
       </c>
@@ -9673,7 +9676,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>26</v>
       </c>
@@ -9700,7 +9703,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>27</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -9750,7 +9753,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>29</v>
       </c>
@@ -9775,7 +9778,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>30</v>
       </c>
@@ -9806,7 +9809,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>31</v>
       </c>
@@ -9837,7 +9840,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>32</v>
       </c>
@@ -9868,7 +9871,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>33</v>
       </c>
@@ -9899,7 +9902,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>36</v>
       </c>
@@ -9932,7 +9935,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>37</v>
       </c>
@@ -9956,13 +9959,13 @@
         <v>155</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>38</v>
       </c>
@@ -9992,7 +9995,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>39</v>
       </c>
@@ -10022,7 +10025,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>42</v>
       </c>
@@ -10049,10 +10052,10 @@
         <v>351</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45</v>
       </c>
@@ -10083,7 +10086,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>46</v>
       </c>
@@ -10114,7 +10117,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>49</v>
       </c>
@@ -10144,7 +10147,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75">
+    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>50</v>
       </c>
@@ -10177,7 +10180,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75">
+    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>51</v>
       </c>
@@ -10207,7 +10210,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75">
+    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>52</v>
       </c>
@@ -10240,7 +10243,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>53</v>
       </c>
@@ -10270,7 +10273,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>56</v>
       </c>
@@ -10300,7 +10303,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>57</v>
       </c>
@@ -10330,7 +10333,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>58</v>
       </c>
@@ -10360,7 +10363,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>59</v>
       </c>
@@ -10390,7 +10393,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>60</v>
       </c>
@@ -10420,7 +10423,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>63</v>
       </c>
@@ -10451,7 +10454,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>64</v>
       </c>
@@ -10482,7 +10485,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>67</v>
       </c>
@@ -10503,19 +10506,19 @@
         <v>111</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>486</v>
       </c>
       <c r="I52" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="J52" s="5" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>68</v>
       </c>
@@ -10527,7 +10530,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>73</v>
@@ -10536,7 +10539,7 @@
         <v>111</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>194</v>
@@ -10545,10 +10548,10 @@
         <v>517</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>69</v>
       </c>
@@ -10560,7 +10563,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>73</v>
@@ -10569,7 +10572,7 @@
         <v>111</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>194</v>
@@ -10578,10 +10581,10 @@
         <v>519</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>70</v>
       </c>
@@ -10593,7 +10596,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>73</v>
@@ -10602,24 +10605,24 @@
         <v>229</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>244</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -10645,12 +10648,12 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
@@ -10675,7 +10678,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>75</v>
       </c>
@@ -10706,7 +10709,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>76</v>
       </c>
@@ -10737,7 +10740,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>77</v>
       </c>
@@ -10768,7 +10771,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>80</v>
       </c>
@@ -10788,19 +10791,19 @@
         <v>111</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>81</v>
       </c>
@@ -10820,20 +10823,20 @@
         <v>111</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and a category code = `laboratory`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>82</v>
       </c>
@@ -10863,7 +10866,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>83</v>
       </c>
@@ -10883,20 +10886,20 @@
         <v>229</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="J64" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>84</v>
       </c>
@@ -10926,7 +10929,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>85</v>
       </c>
@@ -10956,7 +10959,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>88</v>
       </c>
@@ -10989,7 +10992,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>89</v>
       </c>
@@ -11021,7 +11024,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>90</v>
       </c>
@@ -11053,7 +11056,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>91</v>
       </c>
@@ -11085,7 +11088,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>94</v>
       </c>
@@ -11118,7 +11121,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75">
+    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>97</v>
       </c>
@@ -11151,7 +11154,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>100</v>
       </c>
@@ -11171,20 +11174,20 @@
         <v>111</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>101</v>
       </c>
@@ -11204,20 +11207,20 @@
         <v>111</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>300</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>102</v>
       </c>
@@ -11237,7 +11240,7 @@
         <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>303</v>
@@ -11250,7 +11253,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>103</v>
       </c>
@@ -11270,20 +11273,20 @@
         <v>229</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>306</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>104</v>
       </c>
@@ -11313,7 +11316,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>107</v>
       </c>
@@ -11344,7 +11347,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="20.25" customHeight="1">
+    <row r="79" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>108</v>
       </c>
@@ -11373,7 +11376,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>109</v>
       </c>
@@ -11406,7 +11409,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="20.25" customHeight="1">
+    <row r="81" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>110</v>
       </c>
@@ -11439,7 +11442,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>111</v>
       </c>
@@ -11469,7 +11472,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="20.25" customHeight="1">
+    <row r="83" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>112</v>
       </c>
@@ -11500,7 +11503,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
update comment instructions, apply new comments against FHIR-26840
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CB75CF-F7FE-46A2-82F3-C2A4492C5D12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E0BFA7-D34A-4212-8C28-A57175937297}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="690" windowWidth="25200" windowHeight="13425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1249,9 +1249,6 @@
     <t>US Core CareTeam Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</t>
-  </si>
-  <si>
     <t>US Core MedicationStatement Profile</t>
   </si>
   <si>
@@ -1448,9 +1445,6 @@
   </si>
   <si>
     <t>conditionalDelete</t>
-  </si>
-  <si>
-    <t>The MedicationStatement and MedicationRequest resources can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationStatement or a MedicationRequest, then the READ and SEARCH Criteria  **SHALL**  be supported.</t>
   </si>
   <si>
     <t>versioning_conf</t>
@@ -1763,6 +1757,12 @@
   </si>
   <si>
     <t>US Core Pediatric Head Occipital-frontal Circumference Percentile Profile</t>
+  </si>
+  <si>
+    <t>The MedicationRequest resource can represent a medication, using an external reference to a Medication resource. If an external Medication Resource is used in a MedicationRequest, then the READ and SEARCH Criteria  **SHALL**  be supported.</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</t>
   </si>
 </sst>
 </file>
@@ -2257,34 +2257,34 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2292,12 +2292,12 @@
         <v>70</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
@@ -2305,10 +2305,10 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -2320,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="I39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3230,7 +3230,7 @@
         <v>111</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>161</v>
@@ -3266,7 +3266,7 @@
         <v>155</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>151</v>
@@ -3359,7 +3359,7 @@
         <v>351</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3773,7 +3773,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>73</v>
@@ -3785,7 +3785,7 @@
         <v>218</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J51" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified "&amp;SUBSTITUTE(D51,","," and ")</f>
@@ -3804,7 +3804,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>73</v>
@@ -3813,16 +3813,16 @@
         <v>111</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3837,7 +3837,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>73</v>
@@ -3846,16 +3846,16 @@
         <v>111</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3870,7 +3870,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>73</v>
@@ -3879,16 +3879,16 @@
         <v>111</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3903,7 +3903,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>73</v>
@@ -3912,16 +3912,16 @@
         <v>229</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>244</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -3929,7 +3929,7 @@
         <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3948,7 +3948,7 @@
         <v>196</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J56" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -3960,7 +3960,7 @@
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3979,7 +3979,7 @@
         <v>245</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>247</v>
@@ -4086,7 +4086,7 @@
         <v>191</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>251</v>
@@ -4098,13 +4098,13 @@
         <v>111</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>347</v>
@@ -4118,7 +4118,7 @@
         <v>191</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>150</v>
@@ -4130,13 +4130,13 @@
         <v>111</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>233</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -4151,7 +4151,7 @@
         <v>191</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>152</v>
@@ -4181,7 +4181,7 @@
         <v>191</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>203</v>
@@ -4193,13 +4193,13 @@
         <v>229</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>238</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="J64" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -4214,7 +4214,7 @@
         <v>191</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>230</v>
@@ -4244,7 +4244,7 @@
         <v>346</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>121</v>
@@ -4325,7 +4325,7 @@
         <v>255</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>259</v>
@@ -4389,7 +4389,7 @@
         <v>254</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>261</v>
@@ -4481,13 +4481,13 @@
         <v>111</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>301</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J73" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")</f>
@@ -4514,13 +4514,13 @@
         <v>111</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>300</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J74" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B74&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -4547,7 +4547,7 @@
         <v>111</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>303</v>
@@ -4580,13 +4580,13 @@
         <v>229</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>306</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J76" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B76&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -4773,7 +4773,7 @@
         <v>324</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>321</v>
@@ -4803,7 +4803,7 @@
         <v>325</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -4818,7 +4818,7 @@
         <v>266</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>123</v>
@@ -4830,13 +4830,13 @@
         <v>111</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I84" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="J84" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -4875,15 +4875,15 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4891,7 +4891,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1">
@@ -4899,7 +4899,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4907,7 +4907,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4915,7 +4915,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="141" customHeight="1">
@@ -4923,7 +4923,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1">
@@ -4931,7 +4931,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4966,8 +4966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5009,10 +5009,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -5024,10 +5024,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -5039,10 +5039,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -5057,7 +5057,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -5069,10 +5069,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -5087,7 +5087,7 @@
         <v>297</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -5099,10 +5099,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -5129,10 +5129,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -5144,10 +5144,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -5159,10 +5159,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -5174,10 +5174,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -5189,10 +5189,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -5204,25 +5204,25 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -5237,7 +5237,7 @@
         <v>198</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -5249,10 +5249,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -5267,7 +5267,7 @@
         <v>250</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>394</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -5294,10 +5294,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>396</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -5309,10 +5309,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -5324,10 +5324,10 @@
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1">
       <c r="A24" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -5341,7 +5341,7 @@
         <v>197</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -5355,7 +5355,7 @@
         <v>76</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -5366,24 +5366,24 @@
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
@@ -5404,17 +5404,17 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
@@ -5439,49 +5439,49 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>442</v>
       </c>
       <c r="R1" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>343</v>
@@ -5490,10 +5490,10 @@
         <v>344</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>430</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>431</v>
       </c>
       <c r="X1" t="s">
         <v>19</v>
@@ -5512,7 +5512,7 @@
       <c r="R2"/>
       <c r="V2" s="17"/>
       <c r="W2" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="X2" t="s">
         <v>20</v>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="V3" s="17"/>
       <c r="W3" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="17.25" customHeight="1">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="V4" s="17"/>
       <c r="W4" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="17.25" customHeight="1">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="V5" s="17"/>
       <c r="W5" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="X5" t="s">
         <v>24</v>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="V6" s="17"/>
       <c r="W6" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="17.25" customHeight="1">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="V7" s="17"/>
       <c r="W7" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17.25" customHeight="1">
@@ -5589,11 +5589,11 @@
         <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="V8" s="17"/>
       <c r="W8" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17.25" customHeight="1">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="V9" s="17"/>
       <c r="W9" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="17.25" customHeight="1">
@@ -5617,7 +5617,7 @@
       </c>
       <c r="V10" s="17"/>
       <c r="W10" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="17.25" customHeight="1">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="V11" s="17"/>
       <c r="W11" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="17.25" customHeight="1">
@@ -5644,13 +5644,13 @@
     </row>
     <row r="13" spans="1:24" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>435</v>
+        <v>535</v>
       </c>
       <c r="V13" s="17"/>
       <c r="W13" s="17"/>
@@ -5663,32 +5663,32 @@
         <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="U14" s="7" t="s">
         <v>219</v>
       </c>
       <c r="V14" s="17"/>
       <c r="W14" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="V15" s="17"/>
       <c r="W15" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17.25" customHeight="1">
@@ -5700,7 +5700,7 @@
       </c>
       <c r="V16" s="17"/>
       <c r="W16" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="17.25" customHeight="1">
@@ -5722,7 +5722,7 @@
       </c>
       <c r="V18" s="17"/>
       <c r="W18" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="17.25" customHeight="1">
@@ -5757,12 +5757,12 @@
       </c>
       <c r="V21" s="17"/>
       <c r="W21" s="17" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="15">
       <c r="A22" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>73</v>
@@ -5771,7 +5771,7 @@
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="15">
       <c r="A23" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
@@ -5837,10 +5837,10 @@
     </row>
     <row r="2" spans="1:5" ht="90.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>186</v>
@@ -5849,24 +5849,24 @@
         <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="113.25" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5882,7 +5882,7 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5893,7 +5893,7 @@
     <col min="7" max="7" width="35.28515625" customWidth="1"/>
     <col min="8" max="8" width="28.140625" customWidth="1"/>
     <col min="18" max="18" width="8.85546875" style="1"/>
-    <col min="24" max="24" width="8.85546875" style="1"/>
+    <col min="24" max="24" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -5901,76 +5901,76 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" t="s">
         <v>420</v>
       </c>
-      <c r="W1" t="s">
-        <v>421</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -5993,7 +5993,7 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -6111,7 +6111,7 @@
         <v>12</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -6601,7 +6601,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6614,12 +6614,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -6628,7 +6628,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -6637,7 +6637,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -6663,10 +6663,10 @@
   <dimension ref="A1:AB94"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -6744,19 +6744,19 @@
         <v>48</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>49</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>50</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>51</v>
@@ -9458,7 +9458,7 @@
         <v>188</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>73</v>
@@ -9565,7 +9565,7 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>73</v>
@@ -9669,7 +9669,7 @@
         <v>189</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>73</v>
@@ -9771,7 +9771,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>63</v>
@@ -9824,7 +9824,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>94</v>
@@ -9882,7 +9882,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>242</v>

</xml_diff>

<commit_message>
remove narrative from DR
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/uscore-client.xlsx
+++ b/source/source_spreadsheets/uscore-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\US-Core-R4\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEA055E-AA8B-48EA-830A-4A7B6F417B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E20B5C-50C3-40BD-B530-493A6F1E743B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="975" windowWidth="25200" windowHeight="13425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sp_combos!$B$1:$B$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sps!$A$1:$AB$94</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5405,11 +5405,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
@@ -6664,11 +6664,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
@@ -7072,7 +7072,7 @@
         <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>66</v>

</xml_diff>